<commit_message>
Add generated leaderboard data - 2024-04-05T19:20:48
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
@@ -200,7 +200,7 @@
     <t>shivakrishnamur1</t>
   </si>
   <si>
-    <t>44.28%</t>
+    <t>44.36%</t>
   </si>
   <si>
     <t>22R01A66D1</t>
@@ -800,7 +800,7 @@
     <t>cmr_22r01a73b6</t>
   </si>
   <si>
-    <t>29.52%</t>
+    <t>29.56%</t>
   </si>
   <si>
     <t>22R01A7355</t>
@@ -1364,6 +1364,27 @@
     <t>23.46%</t>
   </si>
   <si>
+    <t>22R01A05L5</t>
+  </si>
+  <si>
+    <t>akshay_18229</t>
+  </si>
+  <si>
+    <t>22r01a6ofu</t>
+  </si>
+  <si>
+    <t>Akshay_Kireet</t>
+  </si>
+  <si>
+    <t>a_22r01a05l5</t>
+  </si>
+  <si>
+    <t>KIREET_5L5</t>
+  </si>
+  <si>
+    <t>22.28%</t>
+  </si>
+  <si>
     <t>22R01A05K5</t>
   </si>
   <si>
@@ -1413,27 +1434,6 @@
   </si>
   <si>
     <t>21.56%</t>
-  </si>
-  <si>
-    <t>22R01A05L5</t>
-  </si>
-  <si>
-    <t>akshay_18229</t>
-  </si>
-  <si>
-    <t>22r01a6ofu</t>
-  </si>
-  <si>
-    <t>Akshay_Kireet</t>
-  </si>
-  <si>
-    <t>a_22r01a05l5</t>
-  </si>
-  <si>
-    <t>KIREET_5L5</t>
-  </si>
-  <si>
-    <t>20.73%</t>
   </si>
   <si>
     <t>22R01A0564</t>
@@ -10164,7 +10164,7 @@
         <v>10.0</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>15.0</v>
+        <v>23.0</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>57</v>
@@ -11924,7 +11924,7 @@
         <v>10.0</v>
       </c>
       <c r="G52" s="2" t="n">
-        <v>56.0</v>
+        <v>60.0</v>
       </c>
       <c r="H52" s="2" t="s">
         <v>260</v>
@@ -13719,34 +13719,34 @@
         <v>451</v>
       </c>
       <c r="D93" s="2" t="n">
-        <v>354.0</v>
+        <v>0.0</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>452</v>
       </c>
       <c r="F93" s="2" t="n">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="G93" s="2" t="n">
-        <v>0.0</v>
+        <v>107.0</v>
       </c>
       <c r="H93" s="2" t="s">
         <v>453</v>
       </c>
       <c r="I93" s="2" t="n">
-        <v>1438.0</v>
+        <v>1331.0</v>
       </c>
       <c r="J93" s="2" t="s">
         <v>454</v>
       </c>
       <c r="K93" s="2" t="n">
-        <v>0.0</v>
+        <v>1069.0</v>
       </c>
       <c r="L93" s="2" t="s">
         <v>455</v>
       </c>
       <c r="M93" s="2" t="n">
-        <v>39.0</v>
+        <v>34.0</v>
       </c>
       <c r="N93" s="2" t="s">
         <v>456</v>
@@ -13763,37 +13763,37 @@
         <v>458</v>
       </c>
       <c r="D94" s="2" t="n">
-        <v>345.0</v>
+        <v>354.0</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="F94" s="2" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="G94" s="2" t="n">
-        <v>13.0</v>
+        <v>0.0</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="I94" s="2" t="n">
-        <v>0.0</v>
+        <v>1438.0</v>
       </c>
       <c r="J94" s="2" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="K94" s="2" t="n">
-        <v>1171.0</v>
+        <v>0.0</v>
       </c>
       <c r="L94" s="2" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="M94" s="2" t="n">
         <v>39.0</v>
       </c>
       <c r="N94" s="2" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
     </row>
     <row r="95">
@@ -13801,43 +13801,43 @@
         <v>94.0</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="D95" s="2" t="n">
-        <v>0.0</v>
+        <v>345.0</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="F95" s="2" t="n">
-        <v>27.0</v>
+        <v>10.0</v>
       </c>
       <c r="G95" s="2" t="n">
-        <v>4.0</v>
+        <v>13.0</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="I95" s="2" t="n">
-        <v>1576.0</v>
+        <v>0.0</v>
       </c>
       <c r="J95" s="2" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="K95" s="2" t="n">
-        <v>1197.0</v>
+        <v>1171.0</v>
       </c>
       <c r="L95" s="2" t="s">
         <v>465</v>
       </c>
       <c r="M95" s="2" t="n">
-        <v>4.0</v>
+        <v>39.0</v>
       </c>
       <c r="N95" s="2" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
     </row>
     <row r="96">
@@ -13845,40 +13845,40 @@
         <v>95.0</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="D96" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="F96" s="2" t="n">
-        <v>30.0</v>
+        <v>27.0</v>
       </c>
       <c r="G96" s="2" t="n">
-        <v>107.0</v>
+        <v>4.0</v>
       </c>
       <c r="H96" s="2" t="s">
         <v>470</v>
       </c>
       <c r="I96" s="2" t="n">
-        <v>1331.0</v>
+        <v>1576.0</v>
       </c>
       <c r="J96" s="2" t="s">
         <v>471</v>
       </c>
       <c r="K96" s="2" t="n">
-        <v>1069.0</v>
+        <v>1197.0</v>
       </c>
       <c r="L96" s="2" t="s">
         <v>472</v>
       </c>
       <c r="M96" s="2" t="n">
-        <v>7.0</v>
+        <v>4.0</v>
       </c>
       <c r="N96" s="2" t="s">
         <v>473</v>

</xml_diff>

<commit_message>
Add generated leaderboard data - 2024-04-14T23:07:08
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
@@ -128,6 +128,18 @@
     <t>54.47%</t>
   </si>
   <si>
+    <t>22R01A05Q2</t>
+  </si>
+  <si>
+    <t>22r01a05q2</t>
+  </si>
+  <si>
+    <t>praneetha5q2</t>
+  </si>
+  <si>
+    <t>50.48%</t>
+  </si>
+  <si>
     <t>22R01A0531</t>
   </si>
   <si>
@@ -158,18 +170,6 @@
     <t>49.83%</t>
   </si>
   <si>
-    <t>22R01A05Q2</t>
-  </si>
-  <si>
-    <t>22r01a05q2</t>
-  </si>
-  <si>
-    <t>praneetha5q2</t>
-  </si>
-  <si>
-    <t>48.52%</t>
-  </si>
-  <si>
     <t>22R01A0597</t>
   </si>
   <si>
@@ -206,6 +206,21 @@
     <t>48.28%</t>
   </si>
   <si>
+    <t>22R01A05N4</t>
+  </si>
+  <si>
+    <t>mkeerthi63027</t>
+  </si>
+  <si>
+    <t>mkeerthify</t>
+  </si>
+  <si>
+    <t>keerthi_mangali</t>
+  </si>
+  <si>
+    <t>48.03%</t>
+  </si>
+  <si>
     <t>22R01A05B2</t>
   </si>
   <si>
@@ -239,22 +254,7 @@
     <t>KIREET_5L5</t>
   </si>
   <si>
-    <t>47.28%</t>
-  </si>
-  <si>
-    <t>22R01A05N4</t>
-  </si>
-  <si>
-    <t>mkeerthi63027</t>
-  </si>
-  <si>
-    <t>mkeerthify</t>
-  </si>
-  <si>
-    <t>keerthi_mangali</t>
-  </si>
-  <si>
-    <t>46.67%</t>
+    <t>47.3%</t>
   </si>
   <si>
     <t>22R01A05A1</t>
@@ -710,7 +710,7 @@
     <t>saiteja665</t>
   </si>
   <si>
-    <t>34.35%</t>
+    <t>34.37%</t>
   </si>
   <si>
     <t>22R01A67D1</t>
@@ -917,7 +917,7 @@
     <t>cmr_22r01a73b6</t>
   </si>
   <si>
-    <t>29.77%</t>
+    <t>29.81%</t>
   </si>
   <si>
     <t>22R01A0566</t>
@@ -10000,13 +10000,13 @@
         <v>39</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>779.0</v>
+        <v>816.0</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>60.0</v>
+        <v>0.0</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>0.0</v>
@@ -10015,19 +10015,19 @@
         <v>39</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>1349.0</v>
+        <v>1490.0</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>40</v>
       </c>
       <c r="K8" s="2" t="n">
-        <v>1413.0</v>
+        <v>1050.0</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>39</v>
       </c>
       <c r="M8" s="2" t="n">
-        <v>6.0</v>
+        <v>156.0</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>41</v>
@@ -10044,37 +10044,37 @@
         <v>43</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>624.0</v>
+        <v>779.0</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>60.0</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>1349.0</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="2" t="n">
-        <v>94.0</v>
-      </c>
-      <c r="G9" s="2" t="n">
-        <v>72.0</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" s="2" t="n">
-        <v>1409.0</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="K9" s="2" t="n">
-        <v>1320.0</v>
+        <v>1413.0</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>43</v>
       </c>
       <c r="M9" s="2" t="n">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10">
@@ -10082,40 +10082,40 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>624.0</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>753.0</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="F10" s="2" t="n">
-        <v>0.0</v>
+        <v>94.0</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>0.0</v>
+        <v>72.0</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>49</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>1490.0</v>
+        <v>1409.0</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>50</v>
       </c>
       <c r="K10" s="2" t="n">
-        <v>1050.0</v>
+        <v>1320.0</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>156.0</v>
+        <v>4.0</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>51</v>
@@ -10220,7 +10220,7 @@
         <v>65</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>807.0</v>
+        <v>755.0</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>66</v>
@@ -10232,22 +10232,22 @@
         <v>0.0</v>
       </c>
       <c r="H13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <v>1477.0</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="I13" s="2" t="n">
-        <v>1424.0</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="K13" s="2" t="n">
-        <v>1139.0</v>
+        <v>1092.0</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>65</v>
       </c>
       <c r="M13" s="2" t="n">
-        <v>114.0</v>
+        <v>143.0</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>68</v>
@@ -10264,37 +10264,37 @@
         <v>70</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>660.0</v>
+        <v>807.0</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>127.0</v>
+        <v>0.0</v>
       </c>
       <c r="H14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>1424.0</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="I14" s="2" t="n">
-        <v>1331.0</v>
-      </c>
-      <c r="J14" s="2" t="s">
+      <c r="K14" s="2" t="n">
+        <v>1139.0</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M14" s="2" t="n">
+        <v>114.0</v>
+      </c>
+      <c r="N14" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="K14" s="2" t="n">
-        <v>1102.0</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="M14" s="2" t="n">
-        <v>85.0</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="15">
@@ -10302,40 +10302,40 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>660.0</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="F15" s="2" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>129.0</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D15" s="2" t="n">
-        <v>711.0</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="I15" s="2" t="n">
+        <v>1331.0</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F15" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G15" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H15" s="2" t="s">
+      <c r="K15" s="2" t="n">
+        <v>1102.0</v>
+      </c>
+      <c r="L15" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="I15" s="2" t="n">
-        <v>1477.0</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="K15" s="2" t="n">
-        <v>1092.0</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="M15" s="2" t="n">
-        <v>143.0</v>
+        <v>85.0</v>
       </c>
       <c r="N15" s="2" t="s">
         <v>80</v>
@@ -11637,7 +11637,7 @@
         <v>118.0</v>
       </c>
       <c r="G45" s="2" t="n">
-        <v>116.0</v>
+        <v>118.0</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>230</v>
@@ -12297,7 +12297,7 @@
         <v>10.0</v>
       </c>
       <c r="G60" s="2" t="n">
-        <v>64.0</v>
+        <v>68.0</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>299</v>

</xml_diff>

<commit_message>
Add generated leaderboard data - 2024-04-18T19:16:59
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
@@ -233,6 +233,24 @@
     <t>keerthi_mangali</t>
   </si>
   <si>
+    <t>22R01A66A5</t>
+  </si>
+  <si>
+    <t>22r01a66a5</t>
+  </si>
+  <si>
+    <t>22r01a9x5i</t>
+  </si>
+  <si>
+    <t>shivakrishna21</t>
+  </si>
+  <si>
+    <t>shivakrishnamur1</t>
+  </si>
+  <si>
+    <t>47.32%</t>
+  </si>
+  <si>
     <t>22R01A05L5</t>
   </si>
   <si>
@@ -285,24 +303,6 @@
   </si>
   <si>
     <t>45.26%</t>
-  </si>
-  <si>
-    <t>22R01A66A5</t>
-  </si>
-  <si>
-    <t>22r01a66a5</t>
-  </si>
-  <si>
-    <t>22r01a9x5i</t>
-  </si>
-  <si>
-    <t>shivakrishna21</t>
-  </si>
-  <si>
-    <t>shivakrishnamur1</t>
-  </si>
-  <si>
-    <t>44.75%</t>
   </si>
   <si>
     <t>22R01A67E0</t>
@@ -10311,37 +10311,37 @@
         <v>74</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>660.0</v>
+        <v>709.0</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>75</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>40.0</v>
+        <v>10.0</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>137.0</v>
+        <v>37.0</v>
       </c>
       <c r="H15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I15" s="2" t="n">
+        <v>1511.0</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="I15" s="2" t="n">
-        <v>1331.0</v>
-      </c>
-      <c r="J15" s="2" t="s">
+      <c r="K15" s="2" t="n">
+        <v>1544.0</v>
+      </c>
+      <c r="L15" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="K15" s="2" t="n">
-        <v>1104.0</v>
-      </c>
-      <c r="L15" s="2" t="s">
+      <c r="M15" s="2" t="n">
+        <v>74.0</v>
+      </c>
+      <c r="N15" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="M15" s="2" t="n">
-        <v>85.0</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="16">
@@ -10349,40 +10349,40 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="n">
+        <v>660.0</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D16" s="2" t="n">
-        <v>895.0</v>
-      </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>137.0</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F16" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G16" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H16" s="2" t="s">
+      <c r="I16" s="2" t="n">
+        <v>1331.0</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="I16" s="2" t="n">
-        <v>1475.0</v>
-      </c>
-      <c r="J16" s="2" t="s">
+      <c r="K16" s="2" t="n">
+        <v>1104.0</v>
+      </c>
+      <c r="L16" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="K16" s="2" t="n">
-        <v>1411.0</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="M16" s="2" t="n">
-        <v>1.0</v>
+        <v>85.0</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>85</v>
@@ -10399,7 +10399,7 @@
         <v>87</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>760.0</v>
+        <v>895.0</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>88</v>
@@ -10411,25 +10411,25 @@
         <v>0.0</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="I17" s="2" t="n">
-        <v>1434.0</v>
+        <v>1475.0</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="K17" s="2" t="n">
-        <v>1054.0</v>
+        <v>1411.0</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>87</v>
       </c>
       <c r="M17" s="2" t="n">
-        <v>103.0</v>
+        <v>1.0</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18">
@@ -10437,40 +10437,40 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>709.0</v>
+        <v>760.0</v>
       </c>
       <c r="E18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F18" s="2" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="G18" s="2" t="n">
-        <v>37.0</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="I18" s="2" t="n">
-        <v>1511.0</v>
+        <v>1434.0</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K18" s="2" t="n">
-        <v>1544.0</v>
+        <v>1054.0</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="M18" s="2" t="n">
-        <v>29.0</v>
+        <v>103.0</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>96</v>

</xml_diff>

<commit_message>
Add generated leaderboard data - 2024-04-20T19:23:11
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
@@ -221,7 +221,7 @@
     <t>22r01a05l1</t>
   </si>
   <si>
-    <t>48.17%</t>
+    <t>48.21%</t>
   </si>
   <si>
     <t>22R01A05B2</t>
@@ -272,7 +272,7 @@
     <t>KIREET_5L5</t>
   </si>
   <si>
-    <t>46.65%</t>
+    <t>46.67%</t>
   </si>
   <si>
     <t>22R01A05A1</t>
@@ -428,7 +428,7 @@
     <t>macom_harshita</t>
   </si>
   <si>
-    <t>41.01%</t>
+    <t>41.26%</t>
   </si>
   <si>
     <t>22R01A66E8</t>
@@ -10226,7 +10226,7 @@
         <v>40.0</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>102.0</v>
+        <v>106.0</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>66</v>
@@ -10358,7 +10358,7 @@
         <v>40.0</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>137.0</v>
+        <v>139.0</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>83</v>
@@ -10816,7 +10816,7 @@
         <v>137</v>
       </c>
       <c r="M26" s="2" t="n">
-        <v>36.0</v>
+        <v>41.0</v>
       </c>
       <c r="N26" s="2" t="s">
         <v>138</v>

</xml_diff>

<commit_message>
Add generated leaderboard data - 2024-04-26T19:17:29
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
@@ -143,7 +143,7 @@
     <t>shivakrishnamur1</t>
   </si>
   <si>
-    <t>53.03%</t>
+    <t>53.26%</t>
   </si>
   <si>
     <t>22R01A05L5</t>
@@ -164,7 +164,7 @@
     <t>KIREET_5L5</t>
   </si>
   <si>
-    <t>52.33%</t>
+    <t>52.35%</t>
   </si>
   <si>
     <t>22R01A05L1</t>
@@ -185,7 +185,7 @@
     <t>22r01a05l1</t>
   </si>
   <si>
-    <t>51.37%</t>
+    <t>51.39%</t>
   </si>
   <si>
     <t>22R01A05Q6</t>
@@ -635,7 +635,7 @@
     <t>eshu5886</t>
   </si>
   <si>
-    <t>35.92%</t>
+    <t>35.93%</t>
   </si>
   <si>
     <t>22R01A66F7</t>
@@ -704,7 +704,7 @@
     <t>saiteja665</t>
   </si>
   <si>
-    <t>34.44%</t>
+    <t>34.46%</t>
   </si>
   <si>
     <t>22R01A67D1</t>
@@ -10147,7 +10147,7 @@
         <v>10.0</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>41.0</v>
+        <v>65.0</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>38</v>
@@ -10191,7 +10191,7 @@
         <v>40.0</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>177.0</v>
+        <v>179.0</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>47</v>
@@ -10235,7 +10235,7 @@
         <v>40.0</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>166.0</v>
+        <v>168.0</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>54</v>
@@ -11599,7 +11599,7 @@
         <v>17.0</v>
       </c>
       <c r="G41" s="2" t="n">
-        <v>8.0</v>
+        <v>10.0</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>205</v>
@@ -11775,7 +11775,7 @@
         <v>118.0</v>
       </c>
       <c r="G45" s="2" t="n">
-        <v>128.0</v>
+        <v>130.0</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>228</v>

</xml_diff>

<commit_message>
Add generated leaderboard data - 2024-05-05T19:18:33
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
@@ -113,6 +113,27 @@
     <t>55.56%</t>
   </si>
   <si>
+    <t>22R01A05L1</t>
+  </si>
+  <si>
+    <t>bobbalavarshithreddy</t>
+  </si>
+  <si>
+    <t>22r01aupp6</t>
+  </si>
+  <si>
+    <t>varshith__reddie</t>
+  </si>
+  <si>
+    <t>v22r01a05l1</t>
+  </si>
+  <si>
+    <t>22r01a05l1</t>
+  </si>
+  <si>
+    <t>55.22%</t>
+  </si>
+  <si>
     <t>22R01A05Q6</t>
   </si>
   <si>
@@ -167,27 +188,6 @@
     <t>53.2%</t>
   </si>
   <si>
-    <t>22R01A05L1</t>
-  </si>
-  <si>
-    <t>bobbalavarshithreddy</t>
-  </si>
-  <si>
-    <t>22r01aupp6</t>
-  </si>
-  <si>
-    <t>varshith__reddie</t>
-  </si>
-  <si>
-    <t>v22r01a05l1</t>
-  </si>
-  <si>
-    <t>22r01a05l1</t>
-  </si>
-  <si>
-    <t>52.76%</t>
-  </si>
-  <si>
     <t>22R01A66A5</t>
   </si>
   <si>
@@ -1700,6 +1700,15 @@
     <t>25.76%</t>
   </si>
   <si>
+    <t>22R01A6670</t>
+  </si>
+  <si>
+    <t>varshini_arige</t>
+  </si>
+  <si>
+    <t>25.71%</t>
+  </si>
+  <si>
     <t>22R01A6667</t>
   </si>
   <si>
@@ -1865,15 +1874,6 @@
     <t>24.48%</t>
   </si>
   <si>
-    <t>22R01A6670</t>
-  </si>
-  <si>
-    <t>varshini_arige</t>
-  </si>
-  <si>
-    <t>24.44%</t>
-  </si>
-  <si>
     <t>22R01A7355</t>
   </si>
   <si>
@@ -4100,6 +4100,21 @@
     <t>7.64%</t>
   </si>
   <si>
+    <t>22R01A66A2</t>
+  </si>
+  <si>
+    <t>22r01a66a2</t>
+  </si>
+  <si>
+    <t>22r01az40l</t>
+  </si>
+  <si>
+    <t>a22r01a66a2</t>
+  </si>
+  <si>
+    <t>7.63%</t>
+  </si>
+  <si>
     <t>22R01A7331</t>
   </si>
   <si>
@@ -4968,21 +4983,6 @@
   </si>
   <si>
     <t>6.29%</t>
-  </si>
-  <si>
-    <t>22R01A66A2</t>
-  </si>
-  <si>
-    <t>22r01a66a2</t>
-  </si>
-  <si>
-    <t>22r01az40l</t>
-  </si>
-  <si>
-    <t>a22r01a66a2</t>
-  </si>
-  <si>
-    <t>6.28%</t>
   </si>
   <si>
     <t>22R01A04H1</t>
@@ -10463,37 +10463,37 @@
         <v>34</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>775.0</v>
+        <v>904.0</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>104.0</v>
+        <v>70.0</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>102.0</v>
+        <v>200.0</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>36</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>1371.0</v>
+        <v>1394.0</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>37</v>
       </c>
       <c r="K7" s="2" t="n">
-        <v>1376.0</v>
+        <v>1371.0</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="M7" s="2" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8">
@@ -10501,43 +10501,43 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>779.0</v>
+        <v>775.0</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>104.0</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>102.0</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>1371.0</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>1376.0</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="2" t="n">
-        <v>93.0</v>
-      </c>
-      <c r="G8" s="2" t="n">
-        <v>19.0</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I8" s="2" t="n">
-        <v>1575.0</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K8" s="2" t="n">
-        <v>1320.0</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="M8" s="2" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9">
@@ -10545,40 +10545,40 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>830.0</v>
+        <v>779.0</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>50.0</v>
+        <v>93.0</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>237.0</v>
+        <v>19.0</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>47</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>1322.0</v>
+        <v>1575.0</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K9" s="2" t="n">
-        <v>1141.0</v>
+        <v>1320.0</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>49</v>
       </c>
       <c r="M9" s="2" t="n">
-        <v>85.0</v>
+        <v>0.0</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>50</v>
@@ -10595,7 +10595,7 @@
         <v>52</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>904.0</v>
+        <v>830.0</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>53</v>
@@ -10604,25 +10604,25 @@
         <v>50.0</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>200.0</v>
+        <v>237.0</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>54</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>1394.0</v>
+        <v>1322.0</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>55</v>
       </c>
       <c r="K10" s="2" t="n">
-        <v>1371.0</v>
+        <v>1141.0</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>56</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>0.0</v>
+        <v>85.0</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>57</v>
@@ -15303,16 +15303,16 @@
         <v>563</v>
       </c>
       <c r="D117" s="2" t="n">
-        <v>608.0</v>
+        <v>614.0</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>563</v>
       </c>
       <c r="F117" s="2" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="G117" s="2" t="n">
-        <v>50.0</v>
+        <v>4.0</v>
       </c>
       <c r="H117" s="2" t="s">
         <v>563</v>
@@ -15324,16 +15324,16 @@
         <v>563</v>
       </c>
       <c r="K117" s="2" t="n">
-        <v>1050.0</v>
+        <v>932.0</v>
       </c>
       <c r="L117" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="M117" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N117" s="2" t="s">
         <v>564</v>
-      </c>
-      <c r="M117" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N117" s="2" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="118">
@@ -15341,43 +15341,43 @@
         <v>117.0</v>
       </c>
       <c r="B118" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="C118" s="2" t="s">
         <v>566</v>
       </c>
-      <c r="C118" s="2" t="s">
+      <c r="D118" s="2" t="n">
+        <v>608.0</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="F118" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G118" s="2" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="H118" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="I118" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J118" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="K118" s="2" t="n">
+        <v>1050.0</v>
+      </c>
+      <c r="L118" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="D118" s="2" t="n">
-        <v>354.0</v>
-      </c>
-      <c r="E118" s="2" t="s">
-        <v>567</v>
-      </c>
-      <c r="F118" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G118" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H118" s="2" t="s">
-        <v>567</v>
-      </c>
-      <c r="I118" s="2" t="n">
-        <v>1438.0</v>
-      </c>
-      <c r="J118" s="2" t="s">
-        <v>567</v>
-      </c>
-      <c r="K118" s="2" t="n">
-        <v>887.0</v>
-      </c>
-      <c r="L118" s="2" t="s">
+      <c r="M118" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N118" s="2" t="s">
         <v>568</v>
-      </c>
-      <c r="M118" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N118" s="2" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="119">
@@ -15385,16 +15385,16 @@
         <v>118.0</v>
       </c>
       <c r="B119" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="C119" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="C119" s="2" t="s">
-        <v>571</v>
-      </c>
       <c r="D119" s="2" t="n">
-        <v>635.0</v>
+        <v>354.0</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>198</v>
+        <v>570</v>
       </c>
       <c r="F119" s="2" t="n">
         <v>0.0</v>
@@ -15406,22 +15406,22 @@
         <v>570</v>
       </c>
       <c r="I119" s="2" t="n">
-        <v>0.0</v>
+        <v>1438.0</v>
       </c>
       <c r="J119" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="K119" s="2" t="n">
+        <v>887.0</v>
+      </c>
+      <c r="L119" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="M119" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N119" s="2" t="s">
         <v>572</v>
-      </c>
-      <c r="K119" s="2" t="n">
-        <v>864.0</v>
-      </c>
-      <c r="L119" s="2" t="s">
-        <v>573</v>
-      </c>
-      <c r="M119" s="2" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="N119" s="2" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="120">
@@ -15429,43 +15429,43 @@
         <v>119.0</v>
       </c>
       <c r="B120" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="D120" s="2" t="n">
+        <v>635.0</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F120" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G120" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H120" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="I120" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J120" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="C120" s="2" t="s">
+      <c r="K120" s="2" t="n">
+        <v>864.0</v>
+      </c>
+      <c r="L120" s="2" t="s">
         <v>576</v>
       </c>
-      <c r="D120" s="2" t="n">
-        <v>345.0</v>
-      </c>
-      <c r="E120" s="2" t="s">
+      <c r="M120" s="2" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="N120" s="2" t="s">
         <v>577</v>
-      </c>
-      <c r="F120" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G120" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H120" s="2" t="s">
-        <v>578</v>
-      </c>
-      <c r="I120" s="2" t="n">
-        <v>1422.0</v>
-      </c>
-      <c r="J120" s="2" t="s">
-        <v>578</v>
-      </c>
-      <c r="K120" s="2" t="n">
-        <v>925.0</v>
-      </c>
-      <c r="L120" s="2" t="s">
-        <v>579</v>
-      </c>
-      <c r="M120" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N120" s="2" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="121">
@@ -15473,34 +15473,34 @@
         <v>120.0</v>
       </c>
       <c r="B121" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="D121" s="2" t="n">
+        <v>345.0</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="F121" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G121" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H121" s="2" t="s">
         <v>581</v>
       </c>
-      <c r="C121" s="2" t="s">
-        <v>582</v>
-      </c>
-      <c r="D121" s="2" t="n">
-        <v>357.0</v>
-      </c>
-      <c r="E121" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="F121" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G121" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H121" s="2" t="s">
-        <v>582</v>
-      </c>
       <c r="I121" s="2" t="n">
-        <v>1410.0</v>
+        <v>1422.0</v>
       </c>
       <c r="J121" s="2" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="K121" s="2" t="n">
-        <v>865.0</v>
+        <v>925.0</v>
       </c>
       <c r="L121" s="2" t="s">
         <v>582</v>
@@ -15509,7 +15509,7 @@
         <v>0.0</v>
       </c>
       <c r="N121" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="122">
@@ -15517,43 +15517,43 @@
         <v>121.0</v>
       </c>
       <c r="B122" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C122" s="2" t="s">
         <v>585</v>
       </c>
-      <c r="C122" s="2" t="s">
+      <c r="D122" s="2" t="n">
+        <v>357.0</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F122" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G122" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H122" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="I122" s="2" t="n">
+        <v>1410.0</v>
+      </c>
+      <c r="J122" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="D122" s="2" t="n">
-        <v>611.0</v>
-      </c>
-      <c r="E122" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="F122" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G122" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H122" s="2" t="s">
-        <v>586</v>
-      </c>
-      <c r="I122" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J122" s="2" t="s">
+      <c r="K122" s="2" t="n">
+        <v>865.0</v>
+      </c>
+      <c r="L122" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="M122" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N122" s="2" t="s">
         <v>587</v>
-      </c>
-      <c r="K122" s="2" t="n">
-        <v>1006.0</v>
-      </c>
-      <c r="L122" s="2" t="s">
-        <v>588</v>
-      </c>
-      <c r="M122" s="2" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="N122" s="2" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="123">
@@ -15561,43 +15561,43 @@
         <v>122.0</v>
       </c>
       <c r="B123" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="D123" s="2" t="n">
+        <v>611.0</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F123" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G123" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H123" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="I123" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J123" s="2" t="s">
         <v>590</v>
       </c>
-      <c r="C123" s="2" t="s">
-        <v>591</v>
-      </c>
-      <c r="D123" s="2" t="n">
-        <v>587.0</v>
-      </c>
-      <c r="E123" s="2" t="s">
-        <v>591</v>
-      </c>
-      <c r="F123" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G123" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H123" s="2" t="s">
-        <v>591</v>
-      </c>
-      <c r="I123" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J123" s="2" t="s">
-        <v>592</v>
-      </c>
       <c r="K123" s="2" t="n">
-        <v>1002.0</v>
+        <v>1006.0</v>
       </c>
       <c r="L123" s="2" t="s">
         <v>591</v>
       </c>
       <c r="M123" s="2" t="n">
-        <v>15.0</v>
+        <v>4.0</v>
       </c>
       <c r="N123" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="124">
@@ -15605,16 +15605,16 @@
         <v>123.0</v>
       </c>
       <c r="B124" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="C124" s="2" t="s">
         <v>594</v>
       </c>
-      <c r="C124" s="2" t="s">
-        <v>595</v>
-      </c>
       <c r="D124" s="2" t="n">
-        <v>584.0</v>
+        <v>587.0</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="F124" s="2" t="n">
         <v>0.0</v>
@@ -15623,7 +15623,7 @@
         <v>0.0</v>
       </c>
       <c r="H124" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="I124" s="2" t="n">
         <v>0.0</v>
@@ -15632,16 +15632,16 @@
         <v>595</v>
       </c>
       <c r="K124" s="2" t="n">
-        <v>1130.0</v>
+        <v>1002.0</v>
       </c>
       <c r="L124" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="M124" s="2" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="N124" s="2" t="s">
         <v>596</v>
-      </c>
-      <c r="M124" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N124" s="2" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="125">
@@ -15649,43 +15649,43 @@
         <v>124.0</v>
       </c>
       <c r="B125" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="C125" s="2" t="s">
         <v>598</v>
       </c>
-      <c r="C125" s="2" t="s">
+      <c r="D125" s="2" t="n">
+        <v>584.0</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="F125" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G125" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H125" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="I125" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J125" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="K125" s="2" t="n">
+        <v>1130.0</v>
+      </c>
+      <c r="L125" s="2" t="s">
         <v>599</v>
       </c>
-      <c r="D125" s="2" t="n">
-        <v>595.0</v>
-      </c>
-      <c r="E125" s="2" t="s">
+      <c r="M125" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N125" s="2" t="s">
         <v>600</v>
-      </c>
-      <c r="F125" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G125" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H125" s="2" t="s">
-        <v>601</v>
-      </c>
-      <c r="I125" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J125" s="2" t="s">
-        <v>601</v>
-      </c>
-      <c r="K125" s="2" t="n">
-        <v>1059.0</v>
-      </c>
-      <c r="L125" s="2" t="s">
-        <v>602</v>
-      </c>
-      <c r="M125" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N125" s="2" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="126">
@@ -15693,34 +15693,34 @@
         <v>125.0</v>
       </c>
       <c r="B126" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="D126" s="2" t="n">
+        <v>595.0</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="F126" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G126" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H126" s="2" t="s">
         <v>604</v>
       </c>
-      <c r="C126" s="2" t="s">
-        <v>605</v>
-      </c>
-      <c r="D126" s="2" t="n">
-        <v>598.0</v>
-      </c>
-      <c r="E126" s="2" t="s">
-        <v>606</v>
-      </c>
-      <c r="F126" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G126" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H126" s="2" t="s">
-        <v>607</v>
-      </c>
       <c r="I126" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="J126" s="2" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="K126" s="2" t="n">
-        <v>1036.0</v>
+        <v>1059.0</v>
       </c>
       <c r="L126" s="2" t="s">
         <v>605</v>
@@ -15729,7 +15729,7 @@
         <v>0.0</v>
       </c>
       <c r="N126" s="2" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="127">
@@ -15737,43 +15737,43 @@
         <v>126.0</v>
       </c>
       <c r="B127" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="D127" s="2" t="n">
+        <v>598.0</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="F127" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G127" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H127" s="2" t="s">
         <v>610</v>
       </c>
-      <c r="C127" s="2" t="s">
+      <c r="I127" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J127" s="2" t="s">
         <v>611</v>
       </c>
-      <c r="D127" s="2" t="n">
-        <v>589.0</v>
-      </c>
-      <c r="E127" s="2" t="s">
+      <c r="K127" s="2" t="n">
+        <v>1036.0</v>
+      </c>
+      <c r="L127" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="M127" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N127" s="2" t="s">
         <v>612</v>
-      </c>
-      <c r="F127" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G127" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H127" s="2" t="s">
-        <v>613</v>
-      </c>
-      <c r="I127" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J127" s="2" t="s">
-        <v>614</v>
-      </c>
-      <c r="K127" s="2" t="n">
-        <v>1053.0</v>
-      </c>
-      <c r="L127" s="2" t="s">
-        <v>615</v>
-      </c>
-      <c r="M127" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N127" s="2" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="128">
@@ -15781,34 +15781,34 @@
         <v>127.0</v>
       </c>
       <c r="B128" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="D128" s="2" t="n">
+        <v>589.0</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="F128" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G128" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H128" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="I128" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J128" s="2" t="s">
         <v>617</v>
       </c>
-      <c r="C128" s="2" t="s">
-        <v>618</v>
-      </c>
-      <c r="D128" s="2" t="n">
-        <v>614.0</v>
-      </c>
-      <c r="E128" s="2" t="s">
-        <v>618</v>
-      </c>
-      <c r="F128" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G128" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H128" s="2" t="s">
-        <v>618</v>
-      </c>
-      <c r="I128" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J128" s="2" t="s">
-        <v>618</v>
-      </c>
       <c r="K128" s="2" t="n">
-        <v>932.0</v>
+        <v>1053.0</v>
       </c>
       <c r="L128" s="2" t="s">
         <v>618</v>
@@ -22522,13 +22522,13 @@
         <v>0.0</v>
       </c>
       <c r="E281" s="2" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="F281" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="G281" s="2" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="H281" s="2" t="s">
         <v>1363</v>
@@ -22537,19 +22537,19 @@
         <v>0.0</v>
       </c>
       <c r="J281" s="2" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
       <c r="K281" s="2" t="n">
-        <v>1179.0</v>
+        <v>926.0</v>
       </c>
       <c r="L281" s="2" t="s">
         <v>1363</v>
       </c>
       <c r="M281" s="2" t="n">
-        <v>0.0</v>
+        <v>31.0</v>
       </c>
       <c r="N281" s="2" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="282">
@@ -22557,16 +22557,16 @@
         <v>281.0</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
       <c r="C282" s="2" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="D282" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E282" s="2" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="F282" s="2" t="n">
         <v>0.0</v>
@@ -22575,25 +22575,25 @@
         <v>0.0</v>
       </c>
       <c r="H282" s="2" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="I282" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="J282" s="2" t="s">
+        <v>1369</v>
+      </c>
+      <c r="K282" s="2" t="n">
+        <v>1179.0</v>
+      </c>
+      <c r="L282" s="2" t="s">
         <v>1368</v>
       </c>
-      <c r="K282" s="2" t="n">
-        <v>997.0</v>
-      </c>
-      <c r="L282" s="2" t="s">
-        <v>1367</v>
-      </c>
       <c r="M282" s="2" t="n">
-        <v>23.0</v>
+        <v>0.0</v>
       </c>
       <c r="N282" s="2" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="283">
@@ -22601,16 +22601,16 @@
         <v>282.0</v>
       </c>
       <c r="B283" s="2" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
       <c r="C283" s="2" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="D283" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E283" s="2" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="F283" s="2" t="n">
         <v>0.0</v>
@@ -22619,25 +22619,25 @@
         <v>0.0</v>
       </c>
       <c r="H283" s="2" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="I283" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="J283" s="2" t="s">
+        <v>1373</v>
+      </c>
+      <c r="K283" s="2" t="n">
+        <v>997.0</v>
+      </c>
+      <c r="L283" s="2" t="s">
         <v>1372</v>
       </c>
-      <c r="K283" s="2" t="n">
-        <v>1166.0</v>
-      </c>
-      <c r="L283" s="2" t="s">
-        <v>1371</v>
-      </c>
       <c r="M283" s="2" t="n">
-        <v>0.0</v>
+        <v>23.0</v>
       </c>
       <c r="N283" s="2" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="284">
@@ -22645,43 +22645,43 @@
         <v>283.0</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
       <c r="C284" s="2" t="s">
-        <v>198</v>
+        <v>1376</v>
       </c>
       <c r="D284" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E284" s="2" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
       <c r="F284" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="G284" s="2" t="n">
-        <v>7.0</v>
+        <v>0.0</v>
       </c>
       <c r="H284" s="2" t="s">
-        <v>198</v>
+        <v>1376</v>
       </c>
       <c r="I284" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="J284" s="2" t="s">
+        <v>1377</v>
+      </c>
+      <c r="K284" s="2" t="n">
+        <v>1166.0</v>
+      </c>
+      <c r="L284" s="2" t="s">
         <v>1376</v>
       </c>
-      <c r="K284" s="2" t="n">
-        <v>997.0</v>
-      </c>
-      <c r="L284" s="2" t="s">
-        <v>1375</v>
-      </c>
       <c r="M284" s="2" t="n">
-        <v>20.0</v>
+        <v>0.0</v>
       </c>
       <c r="N284" s="2" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="285">
@@ -22689,10 +22689,10 @@
         <v>284.0</v>
       </c>
       <c r="B285" s="2" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="C285" s="2" t="s">
-        <v>1379</v>
+        <v>198</v>
       </c>
       <c r="D285" s="2" t="n">
         <v>0.0</v>
@@ -22704,10 +22704,10 @@
         <v>0.0</v>
       </c>
       <c r="G285" s="2" t="n">
-        <v>28.0</v>
+        <v>7.0</v>
       </c>
       <c r="H285" s="2" t="s">
-        <v>1379</v>
+        <v>198</v>
       </c>
       <c r="I285" s="2" t="n">
         <v>0.0</v>
@@ -22716,16 +22716,16 @@
         <v>1381</v>
       </c>
       <c r="K285" s="2" t="n">
-        <v>934.0</v>
+        <v>997.0</v>
       </c>
       <c r="L285" s="2" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="M285" s="2" t="n">
-        <v>24.0</v>
+        <v>20.0</v>
       </c>
       <c r="N285" s="2" t="s">
-        <v>1377</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="286">
@@ -22733,22 +22733,22 @@
         <v>285.0</v>
       </c>
       <c r="B286" s="2" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="C286" s="2" t="s">
-        <v>1382</v>
+        <v>1384</v>
       </c>
       <c r="D286" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E286" s="2" t="s">
-        <v>1383</v>
+        <v>1385</v>
       </c>
       <c r="F286" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="G286" s="2" t="n">
-        <v>0.0</v>
+        <v>28.0</v>
       </c>
       <c r="H286" s="2" t="s">
         <v>1384</v>
@@ -22757,19 +22757,19 @@
         <v>0.0</v>
       </c>
       <c r="J286" s="2" t="s">
+        <v>1386</v>
+      </c>
+      <c r="K286" s="2" t="n">
+        <v>934.0</v>
+      </c>
+      <c r="L286" s="2" t="s">
         <v>1384</v>
       </c>
-      <c r="K286" s="2" t="n">
-        <v>1161.0</v>
-      </c>
-      <c r="L286" s="2" t="s">
-        <v>1385</v>
-      </c>
       <c r="M286" s="2" t="n">
-        <v>0.0</v>
+        <v>24.0</v>
       </c>
       <c r="N286" s="2" t="s">
-        <v>1386</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="287">
@@ -22780,7 +22780,7 @@
         <v>1387</v>
       </c>
       <c r="C287" s="2" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="D287" s="2" t="n">
         <v>0.0</v>
@@ -22795,7 +22795,7 @@
         <v>0.0</v>
       </c>
       <c r="H287" s="2" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="I287" s="2" t="n">
         <v>0.0</v>
@@ -22804,16 +22804,16 @@
         <v>1389</v>
       </c>
       <c r="K287" s="2" t="n">
-        <v>971.0</v>
+        <v>1161.0</v>
       </c>
       <c r="L287" s="2" t="s">
-        <v>1388</v>
+        <v>1390</v>
       </c>
       <c r="M287" s="2" t="n">
-        <v>24.0</v>
+        <v>0.0</v>
       </c>
       <c r="N287" s="2" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="288">
@@ -22821,16 +22821,16 @@
         <v>287.0</v>
       </c>
       <c r="B288" s="2" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="C288" s="2" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="D288" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E288" s="2" t="s">
-        <v>198</v>
+        <v>1393</v>
       </c>
       <c r="F288" s="2" t="n">
         <v>0.0</v>
@@ -22848,16 +22848,16 @@
         <v>1394</v>
       </c>
       <c r="K288" s="2" t="n">
-        <v>1141.0</v>
+        <v>971.0</v>
       </c>
       <c r="L288" s="2" t="s">
+        <v>1393</v>
+      </c>
+      <c r="M288" s="2" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="N288" s="2" t="s">
         <v>1395</v>
-      </c>
-      <c r="M288" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N288" s="2" t="s">
-        <v>1396</v>
       </c>
     </row>
     <row r="289">
@@ -22865,43 +22865,43 @@
         <v>288.0</v>
       </c>
       <c r="B289" s="2" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C289" s="2" t="s">
         <v>1397</v>
       </c>
-      <c r="C289" s="2" t="s">
-        <v>198</v>
-      </c>
       <c r="D289" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E289" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F289" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G289" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H289" s="2" t="s">
         <v>1398</v>
       </c>
-      <c r="F289" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G289" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H289" s="2" t="s">
+      <c r="I289" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J289" s="2" t="s">
         <v>1399</v>
-      </c>
-      <c r="I289" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J289" s="2" t="s">
-        <v>1400</v>
       </c>
       <c r="K289" s="2" t="n">
         <v>1141.0</v>
       </c>
       <c r="L289" s="2" t="s">
+        <v>1400</v>
+      </c>
+      <c r="M289" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N289" s="2" t="s">
         <v>1401</v>
-      </c>
-      <c r="M289" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N289" s="2" t="s">
-        <v>1396</v>
       </c>
     </row>
     <row r="290">
@@ -22918,7 +22918,7 @@
         <v>0.0</v>
       </c>
       <c r="E290" s="2" t="s">
-        <v>198</v>
+        <v>1403</v>
       </c>
       <c r="F290" s="2" t="n">
         <v>0.0</v>
@@ -22927,25 +22927,25 @@
         <v>0.0</v>
       </c>
       <c r="H290" s="2" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="I290" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="J290" s="2" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="K290" s="2" t="n">
-        <v>1102.0</v>
+        <v>1141.0</v>
       </c>
       <c r="L290" s="2" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="M290" s="2" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="N290" s="2" t="s">
-        <v>1406</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="291">
@@ -22980,13 +22980,13 @@
         <v>1409</v>
       </c>
       <c r="K291" s="2" t="n">
-        <v>921.0</v>
+        <v>1102.0</v>
       </c>
       <c r="L291" s="2" t="s">
         <v>1410</v>
       </c>
       <c r="M291" s="2" t="n">
-        <v>28.0</v>
+        <v>5.0</v>
       </c>
       <c r="N291" s="2" t="s">
         <v>1411</v>
@@ -23006,16 +23006,16 @@
         <v>0.0</v>
       </c>
       <c r="E292" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F292" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G292" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H292" s="2" t="s">
         <v>1413</v>
-      </c>
-      <c r="F292" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G292" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H292" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="I292" s="2" t="n">
         <v>0.0</v>
@@ -23024,16 +23024,16 @@
         <v>1414</v>
       </c>
       <c r="K292" s="2" t="n">
-        <v>1134.0</v>
+        <v>921.0</v>
       </c>
       <c r="L292" s="2" t="s">
-        <v>198</v>
+        <v>1415</v>
       </c>
       <c r="M292" s="2" t="n">
-        <v>0.0</v>
+        <v>28.0</v>
       </c>
       <c r="N292" s="2" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="293">
@@ -23041,16 +23041,16 @@
         <v>292.0</v>
       </c>
       <c r="B293" s="2" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="C293" s="2" t="s">
-        <v>1416</v>
+        <v>198</v>
       </c>
       <c r="D293" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E293" s="2" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="F293" s="2" t="n">
         <v>0.0</v>
@@ -23059,19 +23059,19 @@
         <v>0.0</v>
       </c>
       <c r="H293" s="2" t="s">
-        <v>1416</v>
+        <v>198</v>
       </c>
       <c r="I293" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="J293" s="2" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="K293" s="2" t="n">
-        <v>1132.0</v>
+        <v>1134.0</v>
       </c>
       <c r="L293" s="2" t="s">
-        <v>1419</v>
+        <v>198</v>
       </c>
       <c r="M293" s="2" t="n">
         <v>0.0</v>
@@ -23088,7 +23088,7 @@
         <v>1421</v>
       </c>
       <c r="C294" s="2" t="s">
-        <v>198</v>
+        <v>1421</v>
       </c>
       <c r="D294" s="2" t="n">
         <v>0.0</v>
@@ -23103,25 +23103,25 @@
         <v>0.0</v>
       </c>
       <c r="H294" s="2" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="I294" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="J294" s="2" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="K294" s="2" t="n">
-        <v>1129.0</v>
+        <v>1132.0</v>
       </c>
       <c r="L294" s="2" t="s">
-        <v>1422</v>
+        <v>1424</v>
       </c>
       <c r="M294" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="N294" s="2" t="s">
-        <v>1423</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="295">
@@ -23129,16 +23129,16 @@
         <v>294.0</v>
       </c>
       <c r="B295" s="2" t="s">
-        <v>1424</v>
+        <v>1426</v>
       </c>
       <c r="C295" s="2" t="s">
-        <v>1425</v>
+        <v>198</v>
       </c>
       <c r="D295" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E295" s="2" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="F295" s="2" t="n">
         <v>0.0</v>
@@ -23147,22 +23147,22 @@
         <v>0.0</v>
       </c>
       <c r="H295" s="2" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="I295" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="J295" s="2" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="K295" s="2" t="n">
-        <v>1046.0</v>
+        <v>1129.0</v>
       </c>
       <c r="L295" s="2" t="s">
         <v>1427</v>
       </c>
       <c r="M295" s="2" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="N295" s="2" t="s">
         <v>1428</v>
@@ -23176,13 +23176,13 @@
         <v>1429</v>
       </c>
       <c r="C296" s="2" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="D296" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E296" s="2" t="s">
-        <v>1429</v>
+        <v>1431</v>
       </c>
       <c r="F296" s="2" t="n">
         <v>0.0</v>
@@ -23191,7 +23191,7 @@
         <v>0.0</v>
       </c>
       <c r="H296" s="2" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="I296" s="2" t="n">
         <v>0.0</v>
@@ -23200,13 +23200,13 @@
         <v>1431</v>
       </c>
       <c r="K296" s="2" t="n">
-        <v>1095.0</v>
+        <v>1046.0</v>
       </c>
       <c r="L296" s="2" t="s">
         <v>1432</v>
       </c>
       <c r="M296" s="2" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="N296" s="2" t="s">
         <v>1433</v>
@@ -23220,13 +23220,13 @@
         <v>1434</v>
       </c>
       <c r="C297" s="2" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="D297" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E297" s="2" t="s">
-        <v>198</v>
+        <v>1434</v>
       </c>
       <c r="F297" s="2" t="n">
         <v>0.0</v>
@@ -23244,16 +23244,16 @@
         <v>1436</v>
       </c>
       <c r="K297" s="2" t="n">
-        <v>1092.0</v>
+        <v>1095.0</v>
       </c>
       <c r="L297" s="2" t="s">
-        <v>1435</v>
+        <v>1437</v>
       </c>
       <c r="M297" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="N297" s="2" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="298">
@@ -23261,16 +23261,16 @@
         <v>297.0</v>
       </c>
       <c r="B298" s="2" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="C298" s="2" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="D298" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E298" s="2" t="s">
-        <v>1439</v>
+        <v>198</v>
       </c>
       <c r="F298" s="2" t="n">
         <v>0.0</v>
@@ -23279,25 +23279,25 @@
         <v>0.0</v>
       </c>
       <c r="H298" s="2" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="I298" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="J298" s="2" t="s">
-        <v>1439</v>
+        <v>1441</v>
       </c>
       <c r="K298" s="2" t="n">
-        <v>1090.0</v>
+        <v>1092.0</v>
       </c>
       <c r="L298" s="2" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="M298" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="N298" s="2" t="s">
-        <v>1440</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="299">
@@ -23305,16 +23305,16 @@
         <v>298.0</v>
       </c>
       <c r="B299" s="2" t="s">
-        <v>1441</v>
+        <v>1443</v>
       </c>
       <c r="C299" s="2" t="s">
-        <v>1442</v>
+        <v>1444</v>
       </c>
       <c r="D299" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E299" s="2" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="F299" s="2" t="n">
         <v>0.0</v>
@@ -23323,7 +23323,7 @@
         <v>0.0</v>
       </c>
       <c r="H299" s="2" t="s">
-        <v>1442</v>
+        <v>1444</v>
       </c>
       <c r="I299" s="2" t="n">
         <v>0.0</v>
@@ -23332,16 +23332,16 @@
         <v>1444</v>
       </c>
       <c r="K299" s="2" t="n">
-        <v>1089.0</v>
+        <v>1090.0</v>
       </c>
       <c r="L299" s="2" t="s">
+        <v>1444</v>
+      </c>
+      <c r="M299" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N299" s="2" t="s">
         <v>1445</v>
-      </c>
-      <c r="M299" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N299" s="2" t="s">
-        <v>1446</v>
       </c>
     </row>
     <row r="300">
@@ -23349,43 +23349,43 @@
         <v>299.0</v>
       </c>
       <c r="B300" s="2" t="s">
+        <v>1446</v>
+      </c>
+      <c r="C300" s="2" t="s">
         <v>1447</v>
       </c>
-      <c r="C300" s="2" t="s">
+      <c r="D300" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E300" s="2" t="s">
         <v>1448</v>
       </c>
-      <c r="D300" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E300" s="2" t="s">
+      <c r="F300" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G300" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H300" s="2" t="s">
+        <v>1447</v>
+      </c>
+      <c r="I300" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J300" s="2" t="s">
         <v>1449</v>
-      </c>
-      <c r="F300" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G300" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H300" s="2" t="s">
-        <v>1450</v>
-      </c>
-      <c r="I300" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J300" s="2" t="s">
-        <v>1451</v>
       </c>
       <c r="K300" s="2" t="n">
         <v>1089.0</v>
       </c>
       <c r="L300" s="2" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="M300" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="N300" s="2" t="s">
-        <v>1446</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="301">
@@ -23393,43 +23393,43 @@
         <v>300.0</v>
       </c>
       <c r="B301" s="2" t="s">
+        <v>1452</v>
+      </c>
+      <c r="C301" s="2" t="s">
         <v>1453</v>
       </c>
-      <c r="C301" s="2" t="s">
+      <c r="D301" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E301" s="2" t="s">
         <v>1454</v>
       </c>
-      <c r="D301" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E301" s="2" t="s">
+      <c r="F301" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G301" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H301" s="2" t="s">
         <v>1455</v>
       </c>
-      <c r="F301" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G301" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H301" s="2" t="s">
+      <c r="I301" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J301" s="2" t="s">
         <v>1456</v>
       </c>
-      <c r="I301" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J301" s="2" t="s">
+      <c r="K301" s="2" t="n">
+        <v>1089.0</v>
+      </c>
+      <c r="L301" s="2" t="s">
         <v>1457</v>
       </c>
-      <c r="K301" s="2" t="n">
-        <v>1057.0</v>
-      </c>
-      <c r="L301" s="2" t="s">
-        <v>1456</v>
-      </c>
       <c r="M301" s="2" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="N301" s="2" t="s">
-        <v>1458</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="302">
@@ -23437,10 +23437,10 @@
         <v>301.0</v>
       </c>
       <c r="B302" s="2" t="s">
+        <v>1458</v>
+      </c>
+      <c r="C302" s="2" t="s">
         <v>1459</v>
-      </c>
-      <c r="C302" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="D302" s="2" t="n">
         <v>0.0</v>
@@ -23461,19 +23461,19 @@
         <v>0.0</v>
       </c>
       <c r="J302" s="2" t="s">
+        <v>1462</v>
+      </c>
+      <c r="K302" s="2" t="n">
+        <v>1057.0</v>
+      </c>
+      <c r="L302" s="2" t="s">
         <v>1461</v>
       </c>
-      <c r="K302" s="2" t="n">
-        <v>1087.0</v>
-      </c>
-      <c r="L302" s="2" t="s">
-        <v>1462</v>
-      </c>
       <c r="M302" s="2" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="N302" s="2" t="s">
-        <v>1458</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="303">
@@ -23481,16 +23481,16 @@
         <v>302.0</v>
       </c>
       <c r="B303" s="2" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="C303" s="2" t="s">
-        <v>1464</v>
+        <v>198</v>
       </c>
       <c r="D303" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E303" s="2" t="s">
-        <v>198</v>
+        <v>1465</v>
       </c>
       <c r="F303" s="2" t="n">
         <v>0.0</v>
@@ -23499,7 +23499,7 @@
         <v>0.0</v>
       </c>
       <c r="H303" s="2" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="I303" s="2" t="n">
         <v>0.0</v>
@@ -23508,16 +23508,16 @@
         <v>1466</v>
       </c>
       <c r="K303" s="2" t="n">
-        <v>994.0</v>
+        <v>1087.0</v>
       </c>
       <c r="L303" s="2" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="M303" s="2" t="n">
-        <v>12.0</v>
+        <v>0.0</v>
       </c>
       <c r="N303" s="2" t="s">
-        <v>1467</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="304">
@@ -23528,13 +23528,13 @@
         <v>1468</v>
       </c>
       <c r="C304" s="2" t="s">
-        <v>198</v>
+        <v>1469</v>
       </c>
       <c r="D304" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E304" s="2" t="s">
-        <v>1469</v>
+        <v>198</v>
       </c>
       <c r="F304" s="2" t="n">
         <v>0.0</v>
@@ -23543,25 +23543,25 @@
         <v>0.0</v>
       </c>
       <c r="H304" s="2" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
       <c r="I304" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="J304" s="2" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="K304" s="2" t="n">
-        <v>1086.0</v>
+        <v>994.0</v>
       </c>
       <c r="L304" s="2" t="s">
-        <v>1469</v>
+        <v>1471</v>
       </c>
       <c r="M304" s="2" t="n">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
       <c r="N304" s="2" t="s">
-        <v>1467</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="305">
@@ -23569,7 +23569,7 @@
         <v>304.0</v>
       </c>
       <c r="B305" s="2" t="s">
-        <v>1471</v>
+        <v>1473</v>
       </c>
       <c r="C305" s="2" t="s">
         <v>198</v>
@@ -23578,7 +23578,7 @@
         <v>0.0</v>
       </c>
       <c r="E305" s="2" t="s">
-        <v>198</v>
+        <v>1474</v>
       </c>
       <c r="F305" s="2" t="n">
         <v>0.0</v>
@@ -23587,25 +23587,25 @@
         <v>0.0</v>
       </c>
       <c r="H305" s="2" t="s">
-        <v>1472</v>
+        <v>1474</v>
       </c>
       <c r="I305" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="J305" s="2" t="s">
-        <v>1473</v>
+        <v>1475</v>
       </c>
       <c r="K305" s="2" t="n">
-        <v>802.0</v>
+        <v>1086.0</v>
       </c>
       <c r="L305" s="2" t="s">
         <v>1474</v>
       </c>
       <c r="M305" s="2" t="n">
-        <v>36.0</v>
+        <v>0.0</v>
       </c>
       <c r="N305" s="2" t="s">
-        <v>1475</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="306">
@@ -23622,16 +23622,16 @@
         <v>0.0</v>
       </c>
       <c r="E306" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F306" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G306" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H306" s="2" t="s">
         <v>1477</v>
-      </c>
-      <c r="F306" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G306" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H306" s="2" t="s">
-        <v>1478</v>
       </c>
       <c r="I306" s="2" t="n">
         <v>0.0</v>
@@ -23640,13 +23640,13 @@
         <v>1478</v>
       </c>
       <c r="K306" s="2" t="n">
-        <v>1076.0</v>
+        <v>802.0</v>
       </c>
       <c r="L306" s="2" t="s">
         <v>1479</v>
       </c>
       <c r="M306" s="2" t="n">
-        <v>0.0</v>
+        <v>36.0</v>
       </c>
       <c r="N306" s="2" t="s">
         <v>1480</v>
@@ -23681,16 +23681,16 @@
         <v>0.0</v>
       </c>
       <c r="J307" s="2" t="s">
+        <v>1483</v>
+      </c>
+      <c r="K307" s="2" t="n">
+        <v>1076.0</v>
+      </c>
+      <c r="L307" s="2" t="s">
         <v>1484</v>
       </c>
-      <c r="K307" s="2" t="n">
-        <v>952.0</v>
-      </c>
-      <c r="L307" s="2" t="s">
-        <v>1481</v>
-      </c>
       <c r="M307" s="2" t="n">
-        <v>16.0</v>
+        <v>0.0</v>
       </c>
       <c r="N307" s="2" t="s">
         <v>1485</v>
@@ -23704,40 +23704,40 @@
         <v>1486</v>
       </c>
       <c r="C308" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D308" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E308" s="2" t="s">
         <v>1487</v>
       </c>
-      <c r="D308" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E308" s="2" t="s">
+      <c r="F308" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G308" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H308" s="2" t="s">
         <v>1488</v>
       </c>
-      <c r="F308" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G308" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H308" s="2" t="s">
+      <c r="I308" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J308" s="2" t="s">
         <v>1489</v>
       </c>
-      <c r="I308" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J308" s="2" t="s">
+      <c r="K308" s="2" t="n">
+        <v>952.0</v>
+      </c>
+      <c r="L308" s="2" t="s">
+        <v>1486</v>
+      </c>
+      <c r="M308" s="2" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="N308" s="2" t="s">
         <v>1490</v>
-      </c>
-      <c r="K308" s="2" t="n">
-        <v>1034.0</v>
-      </c>
-      <c r="L308" s="2" t="s">
-        <v>1487</v>
-      </c>
-      <c r="M308" s="2" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="N308" s="2" t="s">
-        <v>1491</v>
       </c>
     </row>
     <row r="309">
@@ -23745,43 +23745,43 @@
         <v>308.0</v>
       </c>
       <c r="B309" s="2" t="s">
+        <v>1491</v>
+      </c>
+      <c r="C309" s="2" t="s">
         <v>1492</v>
       </c>
-      <c r="C309" s="2" t="s">
+      <c r="D309" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E309" s="2" t="s">
         <v>1493</v>
       </c>
-      <c r="D309" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E309" s="2" t="s">
+      <c r="F309" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G309" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H309" s="2" t="s">
         <v>1494</v>
       </c>
-      <c r="F309" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G309" s="2" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="H309" s="2" t="s">
+      <c r="I309" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J309" s="2" t="s">
         <v>1495</v>
       </c>
-      <c r="I309" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J309" s="2" t="s">
+      <c r="K309" s="2" t="n">
+        <v>1034.0</v>
+      </c>
+      <c r="L309" s="2" t="s">
+        <v>1492</v>
+      </c>
+      <c r="M309" s="2" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="N309" s="2" t="s">
         <v>1496</v>
-      </c>
-      <c r="K309" s="2" t="n">
-        <v>1060.0</v>
-      </c>
-      <c r="L309" s="2" t="s">
-        <v>1493</v>
-      </c>
-      <c r="M309" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N309" s="2" t="s">
-        <v>1497</v>
       </c>
     </row>
     <row r="310">
@@ -23789,25 +23789,25 @@
         <v>309.0</v>
       </c>
       <c r="B310" s="2" t="s">
+        <v>1497</v>
+      </c>
+      <c r="C310" s="2" t="s">
         <v>1498</v>
       </c>
-      <c r="C310" s="2" t="s">
+      <c r="D310" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E310" s="2" t="s">
         <v>1499</v>
       </c>
-      <c r="D310" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E310" s="2" t="s">
+      <c r="F310" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G310" s="2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H310" s="2" t="s">
         <v>1500</v>
-      </c>
-      <c r="F310" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G310" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H310" s="2" t="s">
-        <v>1499</v>
       </c>
       <c r="I310" s="2" t="n">
         <v>0.0</v>
@@ -23816,10 +23816,10 @@
         <v>1501</v>
       </c>
       <c r="K310" s="2" t="n">
-        <v>1058.0</v>
+        <v>1060.0</v>
       </c>
       <c r="L310" s="2" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="M310" s="2" t="n">
         <v>0.0</v>
@@ -23842,13 +23842,13 @@
         <v>0.0</v>
       </c>
       <c r="E311" s="2" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
       <c r="F311" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="G311" s="2" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="H311" s="2" t="s">
         <v>1504</v>
@@ -23857,19 +23857,19 @@
         <v>0.0</v>
       </c>
       <c r="J311" s="2" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
       <c r="K311" s="2" t="n">
-        <v>986.0</v>
+        <v>1058.0</v>
       </c>
       <c r="L311" s="2" t="s">
         <v>1504</v>
       </c>
       <c r="M311" s="2" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="N311" s="2" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="312">
@@ -23877,22 +23877,22 @@
         <v>311.0</v>
       </c>
       <c r="B312" s="2" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
       <c r="C312" s="2" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="D312" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E312" s="2" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
       <c r="F312" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="G312" s="2" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="H312" s="2" t="s">
         <v>1509</v>
@@ -23901,19 +23901,19 @@
         <v>0.0</v>
       </c>
       <c r="J312" s="2" t="s">
+        <v>1510</v>
+      </c>
+      <c r="K312" s="2" t="n">
+        <v>986.0</v>
+      </c>
+      <c r="L312" s="2" t="s">
         <v>1509</v>
       </c>
-      <c r="K312" s="2" t="n">
-        <v>948.0</v>
-      </c>
-      <c r="L312" s="2" t="s">
-        <v>1508</v>
-      </c>
       <c r="M312" s="2" t="n">
-        <v>13.0</v>
+        <v>8.0</v>
       </c>
       <c r="N312" s="2" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="313">
@@ -23921,10 +23921,10 @@
         <v>312.0</v>
       </c>
       <c r="B313" s="2" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
       <c r="C313" s="2" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
       <c r="D313" s="2" t="n">
         <v>0.0</v>
@@ -23945,19 +23945,19 @@
         <v>0.0</v>
       </c>
       <c r="J313" s="2" t="s">
-        <v>1512</v>
+        <v>1514</v>
       </c>
       <c r="K313" s="2" t="n">
-        <v>1048.0</v>
+        <v>948.0</v>
       </c>
       <c r="L313" s="2" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="M313" s="2" t="n">
-        <v>0.0</v>
+        <v>13.0</v>
       </c>
       <c r="N313" s="2" t="s">
-        <v>1510</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="314">
@@ -23965,43 +23965,43 @@
         <v>313.0</v>
       </c>
       <c r="B314" s="2" t="s">
+        <v>1516</v>
+      </c>
+      <c r="C314" s="2" t="s">
+        <v>1517</v>
+      </c>
+      <c r="D314" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E314" s="2" t="s">
+        <v>1518</v>
+      </c>
+      <c r="F314" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G314" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H314" s="2" t="s">
+        <v>1519</v>
+      </c>
+      <c r="I314" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J314" s="2" t="s">
+        <v>1517</v>
+      </c>
+      <c r="K314" s="2" t="n">
+        <v>1048.0</v>
+      </c>
+      <c r="L314" s="2" t="s">
+        <v>1519</v>
+      </c>
+      <c r="M314" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N314" s="2" t="s">
         <v>1515</v>
-      </c>
-      <c r="C314" s="2" t="s">
-        <v>1516</v>
-      </c>
-      <c r="D314" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E314" s="2" t="s">
-        <v>1517</v>
-      </c>
-      <c r="F314" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G314" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H314" s="2" t="s">
-        <v>1515</v>
-      </c>
-      <c r="I314" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J314" s="2" t="s">
-        <v>1518</v>
-      </c>
-      <c r="K314" s="2" t="n">
-        <v>1047.0</v>
-      </c>
-      <c r="L314" s="2" t="s">
-        <v>1516</v>
-      </c>
-      <c r="M314" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N314" s="2" t="s">
-        <v>1510</v>
       </c>
     </row>
     <row r="315">
@@ -24009,43 +24009,43 @@
         <v>314.0</v>
       </c>
       <c r="B315" s="2" t="s">
-        <v>1519</v>
+        <v>1520</v>
       </c>
       <c r="C315" s="2" t="s">
-        <v>198</v>
+        <v>1521</v>
       </c>
       <c r="D315" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E315" s="2" t="s">
+        <v>1522</v>
+      </c>
+      <c r="F315" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G315" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H315" s="2" t="s">
         <v>1520</v>
       </c>
-      <c r="F315" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G315" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H315" s="2" t="s">
+      <c r="I315" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J315" s="2" t="s">
+        <v>1523</v>
+      </c>
+      <c r="K315" s="2" t="n">
+        <v>1047.0</v>
+      </c>
+      <c r="L315" s="2" t="s">
         <v>1521</v>
       </c>
-      <c r="I315" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J315" s="2" t="s">
-        <v>1522</v>
-      </c>
-      <c r="K315" s="2" t="n">
-        <v>1042.0</v>
-      </c>
-      <c r="L315" s="2" t="s">
-        <v>198</v>
-      </c>
       <c r="M315" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="N315" s="2" t="s">
-        <v>1523</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="316">
@@ -24056,13 +24056,13 @@
         <v>1524</v>
       </c>
       <c r="C316" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D316" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E316" s="2" t="s">
         <v>1525</v>
-      </c>
-      <c r="D316" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E316" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="F316" s="2" t="n">
         <v>0.0</v>
@@ -24080,16 +24080,16 @@
         <v>1527</v>
       </c>
       <c r="K316" s="2" t="n">
-        <v>1041.0</v>
+        <v>1042.0</v>
       </c>
       <c r="L316" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="M316" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N316" s="2" t="s">
         <v>1528</v>
-      </c>
-      <c r="M316" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N316" s="2" t="s">
-        <v>1529</v>
       </c>
     </row>
     <row r="317">
@@ -24097,10 +24097,10 @@
         <v>316.0</v>
       </c>
       <c r="B317" s="2" t="s">
+        <v>1529</v>
+      </c>
+      <c r="C317" s="2" t="s">
         <v>1530</v>
-      </c>
-      <c r="C317" s="2" t="s">
-        <v>1531</v>
       </c>
       <c r="D317" s="2" t="n">
         <v>0.0</v>
@@ -24124,16 +24124,16 @@
         <v>1532</v>
       </c>
       <c r="K317" s="2" t="n">
-        <v>1034.0</v>
+        <v>1041.0</v>
       </c>
       <c r="L317" s="2" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="M317" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="N317" s="2" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="318">
@@ -24141,16 +24141,16 @@
         <v>317.0</v>
       </c>
       <c r="B318" s="2" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="C318" s="2" t="s">
-        <v>198</v>
+        <v>1536</v>
       </c>
       <c r="D318" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E318" s="2" t="s">
-        <v>1535</v>
+        <v>198</v>
       </c>
       <c r="F318" s="2" t="n">
         <v>0.0</v>
@@ -24159,25 +24159,25 @@
         <v>0.0</v>
       </c>
       <c r="H318" s="2" t="s">
-        <v>198</v>
+        <v>1536</v>
       </c>
       <c r="I318" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="J318" s="2" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="K318" s="2" t="n">
-        <v>1031.0</v>
+        <v>1034.0</v>
       </c>
       <c r="L318" s="2" t="s">
-        <v>198</v>
+        <v>1537</v>
       </c>
       <c r="M318" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="N318" s="2" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="319">
@@ -24185,7 +24185,7 @@
         <v>318.0</v>
       </c>
       <c r="B319" s="2" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="C319" s="2" t="s">
         <v>198</v>
@@ -24194,7 +24194,7 @@
         <v>0.0</v>
       </c>
       <c r="E319" s="2" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="F319" s="2" t="n">
         <v>0.0</v>
@@ -24203,25 +24203,25 @@
         <v>0.0</v>
       </c>
       <c r="H319" s="2" t="s">
-        <v>1539</v>
+        <v>198</v>
       </c>
       <c r="I319" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="J319" s="2" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="K319" s="2" t="n">
-        <v>922.0</v>
+        <v>1031.0</v>
       </c>
       <c r="L319" s="2" t="s">
-        <v>1539</v>
+        <v>198</v>
       </c>
       <c r="M319" s="2" t="n">
-        <v>14.0</v>
+        <v>0.0</v>
       </c>
       <c r="N319" s="2" t="s">
-        <v>1537</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="320">
@@ -24229,43 +24229,43 @@
         <v>319.0</v>
       </c>
       <c r="B320" s="2" t="s">
-        <v>1541</v>
+        <v>1543</v>
       </c>
       <c r="C320" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D320" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E320" s="2" t="s">
+        <v>1544</v>
+      </c>
+      <c r="F320" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G320" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H320" s="2" t="s">
+        <v>1544</v>
+      </c>
+      <c r="I320" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J320" s="2" t="s">
+        <v>1545</v>
+      </c>
+      <c r="K320" s="2" t="n">
+        <v>922.0</v>
+      </c>
+      <c r="L320" s="2" t="s">
+        <v>1544</v>
+      </c>
+      <c r="M320" s="2" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="N320" s="2" t="s">
         <v>1542</v>
-      </c>
-      <c r="D320" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E320" s="2" t="s">
-        <v>1542</v>
-      </c>
-      <c r="F320" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G320" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H320" s="2" t="s">
-        <v>1542</v>
-      </c>
-      <c r="I320" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J320" s="2" t="s">
-        <v>1543</v>
-      </c>
-      <c r="K320" s="2" t="n">
-        <v>933.0</v>
-      </c>
-      <c r="L320" s="2" t="s">
-        <v>1542</v>
-      </c>
-      <c r="M320" s="2" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="N320" s="2" t="s">
-        <v>1544</v>
       </c>
     </row>
     <row r="321">
@@ -24273,16 +24273,16 @@
         <v>320.0</v>
       </c>
       <c r="B321" s="2" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="C321" s="2" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="D321" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E321" s="2" t="s">
-        <v>198</v>
+        <v>1547</v>
       </c>
       <c r="F321" s="2" t="n">
         <v>0.0</v>
@@ -24297,16 +24297,16 @@
         <v>0.0</v>
       </c>
       <c r="J321" s="2" t="s">
+        <v>1548</v>
+      </c>
+      <c r="K321" s="2" t="n">
+        <v>933.0</v>
+      </c>
+      <c r="L321" s="2" t="s">
         <v>1547</v>
       </c>
-      <c r="K321" s="2" t="n">
-        <v>1020.0</v>
-      </c>
-      <c r="L321" s="2" t="s">
-        <v>1548</v>
-      </c>
       <c r="M321" s="2" t="n">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
       <c r="N321" s="2" t="s">
         <v>1549</v>
@@ -24326,34 +24326,34 @@
         <v>0.0</v>
       </c>
       <c r="E322" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F322" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G322" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H322" s="2" t="s">
         <v>1552</v>
       </c>
-      <c r="F322" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G322" s="2" t="n">
-        <v>85.0</v>
-      </c>
-      <c r="H322" s="2" t="s">
+      <c r="I322" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J322" s="2" t="s">
+        <v>1552</v>
+      </c>
+      <c r="K322" s="2" t="n">
+        <v>1020.0</v>
+      </c>
+      <c r="L322" s="2" t="s">
         <v>1553</v>
       </c>
-      <c r="I322" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J322" s="2" t="s">
-        <v>1551</v>
-      </c>
-      <c r="K322" s="2" t="n">
-        <v>889.0</v>
-      </c>
-      <c r="L322" s="2" t="s">
+      <c r="M322" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N322" s="2" t="s">
         <v>1554</v>
-      </c>
-      <c r="M322" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N322" s="2" t="s">
-        <v>1555</v>
       </c>
     </row>
     <row r="323">
@@ -24361,34 +24361,34 @@
         <v>322.0</v>
       </c>
       <c r="B323" s="2" t="s">
+        <v>1555</v>
+      </c>
+      <c r="C323" s="2" t="s">
         <v>1556</v>
       </c>
-      <c r="C323" s="2" t="s">
-        <v>198</v>
-      </c>
       <c r="D323" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E323" s="2" t="s">
-        <v>198</v>
+        <v>1557</v>
       </c>
       <c r="F323" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="G323" s="2" t="n">
-        <v>0.0</v>
+        <v>85.0</v>
       </c>
       <c r="H323" s="2" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="I323" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="J323" s="2" t="s">
-        <v>1558</v>
+        <v>1556</v>
       </c>
       <c r="K323" s="2" t="n">
-        <v>1018.0</v>
+        <v>889.0</v>
       </c>
       <c r="L323" s="2" t="s">
         <v>1559</v>
@@ -24397,7 +24397,7 @@
         <v>0.0</v>
       </c>
       <c r="N323" s="2" t="s">
-        <v>1555</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="324">
@@ -24405,43 +24405,43 @@
         <v>323.0</v>
       </c>
       <c r="B324" s="2" t="s">
+        <v>1561</v>
+      </c>
+      <c r="C324" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D324" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E324" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F324" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G324" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H324" s="2" t="s">
+        <v>1562</v>
+      </c>
+      <c r="I324" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J324" s="2" t="s">
+        <v>1563</v>
+      </c>
+      <c r="K324" s="2" t="n">
+        <v>1018.0</v>
+      </c>
+      <c r="L324" s="2" t="s">
+        <v>1564</v>
+      </c>
+      <c r="M324" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N324" s="2" t="s">
         <v>1560</v>
-      </c>
-      <c r="C324" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D324" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E324" s="2" t="s">
-        <v>1561</v>
-      </c>
-      <c r="F324" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G324" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H324" s="2" t="s">
-        <v>1560</v>
-      </c>
-      <c r="I324" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J324" s="2" t="s">
-        <v>1562</v>
-      </c>
-      <c r="K324" s="2" t="n">
-        <v>1017.0</v>
-      </c>
-      <c r="L324" s="2" t="s">
-        <v>1561</v>
-      </c>
-      <c r="M324" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N324" s="2" t="s">
-        <v>1563</v>
       </c>
     </row>
     <row r="325">
@@ -24449,25 +24449,25 @@
         <v>324.0</v>
       </c>
       <c r="B325" s="2" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="C325" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D325" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E325" s="2" t="s">
+        <v>1566</v>
+      </c>
+      <c r="F325" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G325" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H325" s="2" t="s">
         <v>1565</v>
-      </c>
-      <c r="D325" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E325" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="F325" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G325" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H325" s="2" t="s">
-        <v>1566</v>
       </c>
       <c r="I325" s="2" t="n">
         <v>0.0</v>
@@ -24476,13 +24476,13 @@
         <v>1567</v>
       </c>
       <c r="K325" s="2" t="n">
-        <v>869.0</v>
+        <v>1017.0</v>
       </c>
       <c r="L325" s="2" t="s">
         <v>1566</v>
       </c>
       <c r="M325" s="2" t="n">
-        <v>19.0</v>
+        <v>0.0</v>
       </c>
       <c r="N325" s="2" t="s">
         <v>1568</v>
@@ -24502,34 +24502,34 @@
         <v>0.0</v>
       </c>
       <c r="E326" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F326" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G326" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H326" s="2" t="s">
         <v>1571</v>
       </c>
-      <c r="F326" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G326" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H326" s="2" t="s">
+      <c r="I326" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J326" s="2" t="s">
         <v>1572</v>
       </c>
-      <c r="I326" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J326" s="2" t="s">
+      <c r="K326" s="2" t="n">
+        <v>869.0</v>
+      </c>
+      <c r="L326" s="2" t="s">
+        <v>1571</v>
+      </c>
+      <c r="M326" s="2" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="N326" s="2" t="s">
         <v>1573</v>
-      </c>
-      <c r="K326" s="2" t="n">
-        <v>1015.0</v>
-      </c>
-      <c r="L326" s="2" t="s">
-        <v>1574</v>
-      </c>
-      <c r="M326" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N326" s="2" t="s">
-        <v>1568</v>
       </c>
     </row>
     <row r="327">
@@ -24537,16 +24537,16 @@
         <v>326.0</v>
       </c>
       <c r="B327" s="2" t="s">
+        <v>1574</v>
+      </c>
+      <c r="C327" s="2" t="s">
         <v>1575</v>
       </c>
-      <c r="C327" s="2" t="s">
+      <c r="D327" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E327" s="2" t="s">
         <v>1576</v>
-      </c>
-      <c r="D327" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E327" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="F327" s="2" t="n">
         <v>0.0</v>
@@ -24564,16 +24564,16 @@
         <v>1578</v>
       </c>
       <c r="K327" s="2" t="n">
-        <v>1009.0</v>
+        <v>1015.0</v>
       </c>
       <c r="L327" s="2" t="s">
-        <v>1575</v>
+        <v>1579</v>
       </c>
       <c r="M327" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="N327" s="2" t="s">
-        <v>1579</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="328">
@@ -24584,13 +24584,13 @@
         <v>1580</v>
       </c>
       <c r="C328" s="2" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="D328" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E328" s="2" t="s">
-        <v>1581</v>
+        <v>198</v>
       </c>
       <c r="F328" s="2" t="n">
         <v>0.0</v>
@@ -24599,16 +24599,16 @@
         <v>0.0</v>
       </c>
       <c r="H328" s="2" t="s">
-        <v>1580</v>
+        <v>1582</v>
       </c>
       <c r="I328" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="J328" s="2" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="K328" s="2" t="n">
-        <v>1008.0</v>
+        <v>1009.0</v>
       </c>
       <c r="L328" s="2" t="s">
         <v>1580</v>
@@ -24617,7 +24617,7 @@
         <v>0.0</v>
       </c>
       <c r="N328" s="2" t="s">
-        <v>1579</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="329">
@@ -24625,16 +24625,16 @@
         <v>328.0</v>
       </c>
       <c r="B329" s="2" t="s">
-        <v>1583</v>
+        <v>1585</v>
       </c>
       <c r="C329" s="2" t="s">
-        <v>198</v>
+        <v>1585</v>
       </c>
       <c r="D329" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E329" s="2" t="s">
-        <v>1584</v>
+        <v>1586</v>
       </c>
       <c r="F329" s="2" t="n">
         <v>0.0</v>
@@ -24643,16 +24643,16 @@
         <v>0.0</v>
       </c>
       <c r="H329" s="2" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="I329" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="J329" s="2" t="s">
-        <v>1584</v>
+        <v>1587</v>
       </c>
       <c r="K329" s="2" t="n">
-        <v>1006.0</v>
+        <v>1008.0</v>
       </c>
       <c r="L329" s="2" t="s">
         <v>1585</v>
@@ -24661,7 +24661,7 @@
         <v>0.0</v>
       </c>
       <c r="N329" s="2" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="330">
@@ -24669,7 +24669,7 @@
         <v>329.0</v>
       </c>
       <c r="B330" s="2" t="s">
-        <v>1587</v>
+        <v>1588</v>
       </c>
       <c r="C330" s="2" t="s">
         <v>198</v>
@@ -24678,7 +24678,7 @@
         <v>0.0</v>
       </c>
       <c r="E330" s="2" t="s">
-        <v>1588</v>
+        <v>1589</v>
       </c>
       <c r="F330" s="2" t="n">
         <v>0.0</v>
@@ -24693,19 +24693,19 @@
         <v>0.0</v>
       </c>
       <c r="J330" s="2" t="s">
+        <v>1589</v>
+      </c>
+      <c r="K330" s="2" t="n">
+        <v>1006.0</v>
+      </c>
+      <c r="L330" s="2" t="s">
         <v>1590</v>
       </c>
-      <c r="K330" s="2" t="n">
-        <v>905.0</v>
-      </c>
-      <c r="L330" s="2" t="s">
+      <c r="M330" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N330" s="2" t="s">
         <v>1591</v>
-      </c>
-      <c r="M330" s="2" t="n">
-        <v>13.0</v>
-      </c>
-      <c r="N330" s="2" t="s">
-        <v>1586</v>
       </c>
     </row>
     <row r="331">
@@ -24716,40 +24716,40 @@
         <v>1592</v>
       </c>
       <c r="C331" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D331" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E331" s="2" t="s">
         <v>1593</v>
       </c>
-      <c r="D331" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E331" s="2" t="s">
+      <c r="F331" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G331" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H331" s="2" t="s">
         <v>1594</v>
       </c>
-      <c r="F331" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G331" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H331" s="2" t="s">
+      <c r="I331" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J331" s="2" t="s">
         <v>1595</v>
       </c>
-      <c r="I331" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J331" s="2" t="s">
+      <c r="K331" s="2" t="n">
+        <v>905.0</v>
+      </c>
+      <c r="L331" s="2" t="s">
         <v>1596</v>
       </c>
-      <c r="K331" s="2" t="n">
-        <v>1004.0</v>
-      </c>
-      <c r="L331" s="2" t="s">
-        <v>1593</v>
-      </c>
       <c r="M331" s="2" t="n">
-        <v>0.0</v>
+        <v>13.0</v>
       </c>
       <c r="N331" s="2" t="s">
-        <v>1597</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="332">
@@ -24757,43 +24757,43 @@
         <v>331.0</v>
       </c>
       <c r="B332" s="2" t="s">
+        <v>1597</v>
+      </c>
+      <c r="C332" s="2" t="s">
         <v>1598</v>
       </c>
-      <c r="C332" s="2" t="s">
+      <c r="D332" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E332" s="2" t="s">
         <v>1599</v>
       </c>
-      <c r="D332" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E332" s="2" t="s">
+      <c r="F332" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G332" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H332" s="2" t="s">
         <v>1600</v>
       </c>
-      <c r="F332" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G332" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H332" s="2" t="s">
+      <c r="I332" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J332" s="2" t="s">
         <v>1601</v>
       </c>
-      <c r="I332" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J332" s="2" t="s">
+      <c r="K332" s="2" t="n">
+        <v>1004.0</v>
+      </c>
+      <c r="L332" s="2" t="s">
+        <v>1598</v>
+      </c>
+      <c r="M332" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N332" s="2" t="s">
         <v>1602</v>
-      </c>
-      <c r="K332" s="2" t="n">
-        <v>1003.0</v>
-      </c>
-      <c r="L332" s="2" t="s">
-        <v>1599</v>
-      </c>
-      <c r="M332" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N332" s="2" t="s">
-        <v>1603</v>
       </c>
     </row>
     <row r="333">
@@ -24801,10 +24801,10 @@
         <v>332.0</v>
       </c>
       <c r="B333" s="2" t="s">
+        <v>1603</v>
+      </c>
+      <c r="C333" s="2" t="s">
         <v>1604</v>
-      </c>
-      <c r="C333" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="D333" s="2" t="n">
         <v>0.0</v>
@@ -24819,25 +24819,25 @@
         <v>0.0</v>
       </c>
       <c r="H333" s="2" t="s">
-        <v>198</v>
+        <v>1606</v>
       </c>
       <c r="I333" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="J333" s="2" t="s">
-        <v>1606</v>
+        <v>1607</v>
       </c>
       <c r="K333" s="2" t="n">
-        <v>1001.0</v>
+        <v>1003.0</v>
       </c>
       <c r="L333" s="2" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="M333" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="N333" s="2" t="s">
-        <v>1607</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="334">
@@ -24845,34 +24845,34 @@
         <v>333.0</v>
       </c>
       <c r="B334" s="2" t="s">
-        <v>1608</v>
+        <v>1609</v>
       </c>
       <c r="C334" s="2" t="s">
-        <v>1609</v>
+        <v>198</v>
       </c>
       <c r="D334" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E334" s="2" t="s">
-        <v>1609</v>
+        <v>1610</v>
       </c>
       <c r="F334" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="G334" s="2" t="n">
-        <v>12.0</v>
+        <v>0.0</v>
       </c>
       <c r="H334" s="2" t="s">
-        <v>1609</v>
+        <v>198</v>
       </c>
       <c r="I334" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="J334" s="2" t="s">
-        <v>1609</v>
+        <v>1611</v>
       </c>
       <c r="K334" s="2" t="n">
-        <v>982.0</v>
+        <v>1001.0</v>
       </c>
       <c r="L334" s="2" t="s">
         <v>1610</v>
@@ -24881,7 +24881,7 @@
         <v>0.0</v>
       </c>
       <c r="N334" s="2" t="s">
-        <v>1607</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="335">
@@ -24889,43 +24889,43 @@
         <v>334.0</v>
       </c>
       <c r="B335" s="2" t="s">
-        <v>1611</v>
+        <v>1613</v>
       </c>
       <c r="C335" s="2" t="s">
-        <v>198</v>
+        <v>1614</v>
       </c>
       <c r="D335" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E335" s="2" t="s">
-        <v>198</v>
+        <v>1614</v>
       </c>
       <c r="F335" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="G335" s="2" t="n">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
       <c r="H335" s="2" t="s">
+        <v>1614</v>
+      </c>
+      <c r="I335" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J335" s="2" t="s">
+        <v>1614</v>
+      </c>
+      <c r="K335" s="2" t="n">
+        <v>982.0</v>
+      </c>
+      <c r="L335" s="2" t="s">
+        <v>1615</v>
+      </c>
+      <c r="M335" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N335" s="2" t="s">
         <v>1612</v>
-      </c>
-      <c r="I335" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J335" s="2" t="s">
-        <v>1613</v>
-      </c>
-      <c r="K335" s="2" t="n">
-        <v>1000.0</v>
-      </c>
-      <c r="L335" s="2" t="s">
-        <v>1614</v>
-      </c>
-      <c r="M335" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N335" s="2" t="s">
-        <v>1615</v>
       </c>
     </row>
     <row r="336">
@@ -24936,13 +24936,13 @@
         <v>1616</v>
       </c>
       <c r="C336" s="2" t="s">
-        <v>1617</v>
+        <v>198</v>
       </c>
       <c r="D336" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E336" s="2" t="s">
-        <v>1617</v>
+        <v>198</v>
       </c>
       <c r="F336" s="2" t="n">
         <v>0.0</v>
@@ -24957,19 +24957,19 @@
         <v>0.0</v>
       </c>
       <c r="J336" s="2" t="s">
-        <v>1617</v>
+        <v>1618</v>
       </c>
       <c r="K336" s="2" t="n">
-        <v>998.0</v>
+        <v>1000.0</v>
       </c>
       <c r="L336" s="2" t="s">
-        <v>1617</v>
+        <v>1619</v>
       </c>
       <c r="M336" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="N336" s="2" t="s">
-        <v>1618</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="337">
@@ -24977,16 +24977,16 @@
         <v>336.0</v>
       </c>
       <c r="B337" s="2" t="s">
-        <v>1619</v>
+        <v>1621</v>
       </c>
       <c r="C337" s="2" t="s">
-        <v>1620</v>
+        <v>1622</v>
       </c>
       <c r="D337" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E337" s="2" t="s">
-        <v>1621</v>
+        <v>1622</v>
       </c>
       <c r="F337" s="2" t="n">
         <v>0.0</v>
@@ -25001,19 +25001,19 @@
         <v>0.0</v>
       </c>
       <c r="J337" s="2" t="s">
+        <v>1622</v>
+      </c>
+      <c r="K337" s="2" t="n">
+        <v>998.0</v>
+      </c>
+      <c r="L337" s="2" t="s">
+        <v>1622</v>
+      </c>
+      <c r="M337" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N337" s="2" t="s">
         <v>1623</v>
-      </c>
-      <c r="K337" s="2" t="n">
-        <v>902.0</v>
-      </c>
-      <c r="L337" s="2" t="s">
-        <v>1620</v>
-      </c>
-      <c r="M337" s="2" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="N337" s="2" t="s">
-        <v>1624</v>
       </c>
     </row>
     <row r="338">
@@ -25021,17 +25021,17 @@
         <v>337.0</v>
       </c>
       <c r="B338" s="2" t="s">
+        <v>1624</v>
+      </c>
+      <c r="C338" s="2" t="s">
         <v>1625</v>
       </c>
-      <c r="C338" s="2" t="s">
+      <c r="D338" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E338" s="2" t="s">
         <v>1626</v>
       </c>
-      <c r="D338" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E338" s="2" t="s">
-        <v>198</v>
-      </c>
       <c r="F338" s="2" t="n">
         <v>0.0</v>
       </c>
@@ -25039,25 +25039,25 @@
         <v>0.0</v>
       </c>
       <c r="H338" s="2" t="s">
-        <v>198</v>
+        <v>1627</v>
       </c>
       <c r="I338" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="J338" s="2" t="s">
-        <v>1627</v>
+        <v>1628</v>
       </c>
       <c r="K338" s="2" t="n">
-        <v>993.0</v>
+        <v>902.0</v>
       </c>
       <c r="L338" s="2" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="M338" s="2" t="n">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
       <c r="N338" s="2" t="s">
-        <v>1628</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="339">
@@ -25065,10 +25065,10 @@
         <v>338.0</v>
       </c>
       <c r="B339" s="2" t="s">
-        <v>1629</v>
+        <v>1630</v>
       </c>
       <c r="C339" s="2" t="s">
-        <v>1630</v>
+        <v>1631</v>
       </c>
       <c r="D339" s="2" t="n">
         <v>0.0</v>
@@ -25083,7 +25083,7 @@
         <v>0.0</v>
       </c>
       <c r="H339" s="2" t="s">
-        <v>1631</v>
+        <v>198</v>
       </c>
       <c r="I339" s="2" t="n">
         <v>0.0</v>
@@ -25092,10 +25092,10 @@
         <v>1632</v>
       </c>
       <c r="K339" s="2" t="n">
-        <v>991.0</v>
+        <v>993.0</v>
       </c>
       <c r="L339" s="2" t="s">
-        <v>1630</v>
+        <v>1631</v>
       </c>
       <c r="M339" s="2" t="n">
         <v>0.0</v>
@@ -25118,28 +25118,28 @@
         <v>0.0</v>
       </c>
       <c r="E340" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F340" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G340" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H340" s="2" t="s">
         <v>1636</v>
       </c>
-      <c r="F340" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G340" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H340" s="2" t="s">
+      <c r="I340" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J340" s="2" t="s">
         <v>1637</v>
       </c>
-      <c r="I340" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J340" s="2" t="s">
+      <c r="K340" s="2" t="n">
+        <v>991.0</v>
+      </c>
+      <c r="L340" s="2" t="s">
         <v>1635</v>
-      </c>
-      <c r="K340" s="2" t="n">
-        <v>990.0</v>
-      </c>
-      <c r="L340" s="2" t="s">
-        <v>1637</v>
       </c>
       <c r="M340" s="2" t="n">
         <v>0.0</v>
@@ -25171,7 +25171,7 @@
         <v>0.0</v>
       </c>
       <c r="H341" s="2" t="s">
-        <v>1640</v>
+        <v>1642</v>
       </c>
       <c r="I341" s="2" t="n">
         <v>0.0</v>
@@ -25189,7 +25189,7 @@
         <v>0.0</v>
       </c>
       <c r="N341" s="2" t="s">
-        <v>1638</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="342">
@@ -25197,16 +25197,16 @@
         <v>341.0</v>
       </c>
       <c r="B342" s="2" t="s">
-        <v>1643</v>
+        <v>1644</v>
       </c>
       <c r="C342" s="2" t="s">
-        <v>198</v>
+        <v>1645</v>
       </c>
       <c r="D342" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E342" s="2" t="s">
-        <v>198</v>
+        <v>1646</v>
       </c>
       <c r="F342" s="2" t="n">
         <v>0.0</v>
@@ -25215,7 +25215,7 @@
         <v>0.0</v>
       </c>
       <c r="H342" s="2" t="s">
-        <v>1644</v>
+        <v>1645</v>
       </c>
       <c r="I342" s="2" t="n">
         <v>0.0</v>
@@ -25224,16 +25224,16 @@
         <v>1645</v>
       </c>
       <c r="K342" s="2" t="n">
-        <v>979.0</v>
+        <v>990.0</v>
       </c>
       <c r="L342" s="2" t="s">
-        <v>198</v>
+        <v>1647</v>
       </c>
       <c r="M342" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="N342" s="2" t="s">
-        <v>1646</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="343">
@@ -25241,10 +25241,10 @@
         <v>342.0</v>
       </c>
       <c r="B343" s="2" t="s">
-        <v>1647</v>
+        <v>1648</v>
       </c>
       <c r="C343" s="2" t="s">
-        <v>1648</v>
+        <v>198</v>
       </c>
       <c r="D343" s="2" t="n">
         <v>0.0</v>
@@ -25265,13 +25265,13 @@
         <v>0.0</v>
       </c>
       <c r="J343" s="2" t="s">
-        <v>1649</v>
+        <v>1650</v>
       </c>
       <c r="K343" s="2" t="n">
-        <v>973.0</v>
+        <v>979.0</v>
       </c>
       <c r="L343" s="2" t="s">
-        <v>1650</v>
+        <v>198</v>
       </c>
       <c r="M343" s="2" t="n">
         <v>0.0</v>
@@ -25294,31 +25294,31 @@
         <v>0.0</v>
       </c>
       <c r="E344" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F344" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G344" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H344" s="2" t="s">
         <v>1654</v>
       </c>
-      <c r="F344" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G344" s="2" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="H344" s="2" t="s">
-        <v>1653</v>
-      </c>
       <c r="I344" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="J344" s="2" t="s">
+        <v>1654</v>
+      </c>
+      <c r="K344" s="2" t="n">
+        <v>973.0</v>
+      </c>
+      <c r="L344" s="2" t="s">
         <v>1655</v>
       </c>
-      <c r="K344" s="2" t="n">
-        <v>926.0</v>
-      </c>
-      <c r="L344" s="2" t="s">
-        <v>1653</v>
-      </c>
       <c r="M344" s="2" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="N344" s="2" t="s">
         <v>1656</v>
@@ -31316,13 +31316,13 @@
         <v>2251</v>
       </c>
       <c r="C481" s="2" t="s">
-        <v>1483</v>
+        <v>1488</v>
       </c>
       <c r="D481" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E481" s="2" t="s">
-        <v>1483</v>
+        <v>1488</v>
       </c>
       <c r="F481" s="2" t="n">
         <v>0.0</v>
@@ -42419,7 +42419,7 @@
         <v>0.0</v>
       </c>
       <c r="H733" s="2" t="s">
-        <v>1605</v>
+        <v>1610</v>
       </c>
       <c r="I733" s="2" t="n">
         <v>0.0</v>

</xml_diff>

<commit_message>
Add generated leaderboard data - 2024-05-14T19:16:35
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
@@ -194,6 +194,24 @@
     <t>56.47%</t>
   </si>
   <si>
+    <t>22R01A05Q6</t>
+  </si>
+  <si>
+    <t>22r01a05q6</t>
+  </si>
+  <si>
+    <t>22r01a0tkh</t>
+  </si>
+  <si>
+    <t>22R01A05W6</t>
+  </si>
+  <si>
+    <t>shahid24</t>
+  </si>
+  <si>
+    <t>56.27%</t>
+  </si>
+  <si>
     <t>22R01A66D5</t>
   </si>
   <si>
@@ -206,25 +224,7 @@
     <t>Sakethreddy168</t>
   </si>
   <si>
-    <t>56.33%</t>
-  </si>
-  <si>
-    <t>22R01A05Q6</t>
-  </si>
-  <si>
-    <t>22r01a05q6</t>
-  </si>
-  <si>
-    <t>22r01a0tkh</t>
-  </si>
-  <si>
-    <t>22R01A05W6</t>
-  </si>
-  <si>
-    <t>shahid24</t>
-  </si>
-  <si>
-    <t>56.25%</t>
+    <t>54.19%</t>
   </si>
   <si>
     <t>22R01A0531</t>
@@ -281,7 +281,7 @@
     <t>koushikpatel</t>
   </si>
   <si>
-    <t>49.25%</t>
+    <t>49.31%</t>
   </si>
   <si>
     <t>22R01A05A1</t>
@@ -3965,6 +3965,21 @@
     <t>8.58%</t>
   </si>
   <si>
+    <t>22R01A66A2</t>
+  </si>
+  <si>
+    <t>22r01a66a2</t>
+  </si>
+  <si>
+    <t>22r01az40l</t>
+  </si>
+  <si>
+    <t>a22r01a66a2</t>
+  </si>
+  <si>
+    <t>8.57%</t>
+  </si>
+  <si>
     <t>22R01A05C3</t>
   </si>
   <si>
@@ -4073,21 +4088,6 @@
     <t>22r01a6644</t>
   </si>
   <si>
-    <t>22R01A66A2</t>
-  </si>
-  <si>
-    <t>22r01a66a2</t>
-  </si>
-  <si>
-    <t>22r01az40l</t>
-  </si>
-  <si>
-    <t>a22r01a66a2</t>
-  </si>
-  <si>
-    <t>8.13%</t>
-  </si>
-  <si>
     <t>22R01A6211</t>
   </si>
   <si>
@@ -4892,7 +4892,7 @@
     <t>sonikamogili</t>
   </si>
   <si>
-    <t>6.54%</t>
+    <t>6.58%</t>
   </si>
   <si>
     <t>22R01A6679</t>
@@ -10729,37 +10729,37 @@
         <v>61</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>779.0</v>
+        <v>776.0</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>62</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>103.0</v>
+        <v>104.0</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>19.0</v>
+        <v>106.0</v>
       </c>
       <c r="H11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>1371.0</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>1399.0</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I11" s="2" t="n">
-        <v>1575.0</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="K11" s="2" t="n">
-        <v>1379.0</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="M11" s="2" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12">
@@ -10767,40 +10767,40 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>776.0</v>
+        <v>779.0</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F12" s="2" t="n">
-        <v>104.0</v>
-      </c>
-      <c r="G12" s="2" t="n">
-        <v>104.0</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="I12" s="2" t="n">
-        <v>1371.0</v>
+        <v>1575.0</v>
       </c>
       <c r="J12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K12" s="2" t="n">
+        <v>1049.0</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="K12" s="2" t="n">
-        <v>1399.0</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="M12" s="2" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>70</v>
@@ -10958,7 +10958,7 @@
         <v>0.0</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>21.0</v>
+        <v>27.0</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>87</v>
@@ -22260,13 +22260,13 @@
         <v>0.0</v>
       </c>
       <c r="E273" s="2" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="F273" s="2" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="G273" s="2" t="n">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
       <c r="H273" s="2" t="s">
         <v>1318</v>
@@ -22275,19 +22275,19 @@
         <v>0.0</v>
       </c>
       <c r="J273" s="2" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="K273" s="2" t="n">
-        <v>1130.0</v>
+        <v>922.0</v>
       </c>
       <c r="L273" s="2" t="s">
         <v>1318</v>
       </c>
       <c r="M273" s="2" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="N273" s="2" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="274">
@@ -22295,19 +22295,19 @@
         <v>273.0</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
       <c r="C274" s="2" t="s">
-        <v>205</v>
+        <v>1323</v>
       </c>
       <c r="D274" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E274" s="2" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="F274" s="2" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="G274" s="2" t="n">
         <v>0.0</v>
@@ -22316,13 +22316,13 @@
         <v>1323</v>
       </c>
       <c r="I274" s="2" t="n">
-        <v>1358.0</v>
+        <v>0.0</v>
       </c>
       <c r="J274" s="2" t="s">
         <v>1324</v>
       </c>
       <c r="K274" s="2" t="n">
-        <v>0.0</v>
+        <v>1130.0</v>
       </c>
       <c r="L274" s="2" t="s">
         <v>1323</v>
@@ -22342,7 +22342,7 @@
         <v>1326</v>
       </c>
       <c r="C275" s="2" t="s">
-        <v>1327</v>
+        <v>205</v>
       </c>
       <c r="D275" s="2" t="n">
         <v>0.0</v>
@@ -22357,22 +22357,22 @@
         <v>0.0</v>
       </c>
       <c r="H275" s="2" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="I275" s="2" t="n">
-        <v>0.0</v>
+        <v>1358.0</v>
       </c>
       <c r="J275" s="2" t="s">
+        <v>1329</v>
+      </c>
+      <c r="K275" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L275" s="2" t="s">
         <v>1328</v>
       </c>
-      <c r="K275" s="2" t="n">
-        <v>1023.0</v>
-      </c>
-      <c r="L275" s="2" t="s">
-        <v>1329</v>
-      </c>
       <c r="M275" s="2" t="n">
-        <v>35.0</v>
+        <v>0.0</v>
       </c>
       <c r="N275" s="2" t="s">
         <v>1330</v>
@@ -22392,7 +22392,7 @@
         <v>0.0</v>
       </c>
       <c r="E276" s="2" t="s">
-        <v>205</v>
+        <v>1332</v>
       </c>
       <c r="F276" s="2" t="n">
         <v>0.0</v>
@@ -22401,7 +22401,7 @@
         <v>0.0</v>
       </c>
       <c r="H276" s="2" t="s">
-        <v>205</v>
+        <v>1332</v>
       </c>
       <c r="I276" s="2" t="n">
         <v>0.0</v>
@@ -22410,16 +22410,16 @@
         <v>1333</v>
       </c>
       <c r="K276" s="2" t="n">
-        <v>1171.0</v>
+        <v>1023.0</v>
       </c>
       <c r="L276" s="2" t="s">
-        <v>1331</v>
+        <v>1334</v>
       </c>
       <c r="M276" s="2" t="n">
-        <v>14.0</v>
+        <v>35.0</v>
       </c>
       <c r="N276" s="2" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="277">
@@ -22427,19 +22427,19 @@
         <v>276.0</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="C277" s="2" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="D277" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E277" s="2" t="s">
-        <v>1337</v>
+        <v>205</v>
       </c>
       <c r="F277" s="2" t="n">
-        <v>20.0</v>
+        <v>0.0</v>
       </c>
       <c r="G277" s="2" t="n">
         <v>0.0</v>
@@ -22454,13 +22454,13 @@
         <v>1338</v>
       </c>
       <c r="K277" s="2" t="n">
-        <v>889.0</v>
+        <v>1171.0</v>
       </c>
       <c r="L277" s="2" t="s">
         <v>1336</v>
       </c>
       <c r="M277" s="2" t="n">
-        <v>0.0</v>
+        <v>14.0</v>
       </c>
       <c r="N277" s="2" t="s">
         <v>1339</v>
@@ -22483,31 +22483,31 @@
         <v>1342</v>
       </c>
       <c r="F278" s="2" t="n">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="G278" s="2" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="H278" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I278" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J278" s="2" t="s">
         <v>1343</v>
       </c>
-      <c r="I278" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J278" s="2" t="s">
+      <c r="K278" s="2" t="n">
+        <v>889.0</v>
+      </c>
+      <c r="L278" s="2" t="s">
         <v>1341</v>
       </c>
-      <c r="K278" s="2" t="n">
-        <v>935.0</v>
-      </c>
-      <c r="L278" s="2" t="s">
+      <c r="M278" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N278" s="2" t="s">
         <v>1344</v>
-      </c>
-      <c r="M278" s="2" t="n">
-        <v>42.0</v>
-      </c>
-      <c r="N278" s="2" t="s">
-        <v>1345</v>
       </c>
     </row>
     <row r="279">
@@ -22515,10 +22515,10 @@
         <v>278.0</v>
       </c>
       <c r="B279" s="2" t="s">
+        <v>1345</v>
+      </c>
+      <c r="C279" s="2" t="s">
         <v>1346</v>
-      </c>
-      <c r="C279" s="2" t="s">
-        <v>1347</v>
       </c>
       <c r="D279" s="2" t="n">
         <v>0.0</v>
@@ -22533,25 +22533,25 @@
         <v>5.0</v>
       </c>
       <c r="H279" s="2" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="I279" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="J279" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="K279" s="2" t="n">
-        <v>904.0</v>
+        <v>935.0</v>
       </c>
       <c r="L279" s="2" t="s">
-        <v>1347</v>
+        <v>1349</v>
       </c>
       <c r="M279" s="2" t="n">
-        <v>46.0</v>
+        <v>42.0</v>
       </c>
       <c r="N279" s="2" t="s">
-        <v>1345</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="280">
@@ -22559,22 +22559,22 @@
         <v>279.0</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>1349</v>
+        <v>1351</v>
       </c>
       <c r="C280" s="2" t="s">
-        <v>1350</v>
+        <v>1352</v>
       </c>
       <c r="D280" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E280" s="2" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="F280" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="G280" s="2" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="H280" s="2" t="s">
         <v>1352</v>
@@ -22583,19 +22583,19 @@
         <v>0.0</v>
       </c>
       <c r="J280" s="2" t="s">
-        <v>1350</v>
+        <v>1353</v>
       </c>
       <c r="K280" s="2" t="n">
-        <v>1119.0</v>
+        <v>904.0</v>
       </c>
       <c r="L280" s="2" t="s">
         <v>1352</v>
       </c>
       <c r="M280" s="2" t="n">
-        <v>19.0</v>
+        <v>46.0</v>
       </c>
       <c r="N280" s="2" t="s">
-        <v>1345</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="281">
@@ -22603,43 +22603,43 @@
         <v>280.0</v>
       </c>
       <c r="B281" s="2" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="C281" s="2" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
       <c r="D281" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E281" s="2" t="s">
+        <v>1356</v>
+      </c>
+      <c r="F281" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G281" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H281" s="2" t="s">
+        <v>1357</v>
+      </c>
+      <c r="I281" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J281" s="2" t="s">
         <v>1355</v>
       </c>
-      <c r="F281" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G281" s="2" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="H281" s="2" t="s">
-        <v>1354</v>
-      </c>
-      <c r="I281" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J281" s="2" t="s">
-        <v>1356</v>
-      </c>
       <c r="K281" s="2" t="n">
-        <v>922.0</v>
+        <v>1119.0</v>
       </c>
       <c r="L281" s="2" t="s">
-        <v>1354</v>
+        <v>1357</v>
       </c>
       <c r="M281" s="2" t="n">
-        <v>41.0</v>
+        <v>19.0</v>
       </c>
       <c r="N281" s="2" t="s">
-        <v>1357</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="282">
@@ -25082,7 +25082,7 @@
         <v>0.0</v>
       </c>
       <c r="G337" s="2" t="n">
-        <v>12.0</v>
+        <v>16.0</v>
       </c>
       <c r="H337" s="2" t="s">
         <v>1624</v>

</xml_diff>

<commit_message>
Add generated leaderboard data - 2024-05-24T19:16:47
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
@@ -113,7 +113,7 @@
     <t>sellilavanya</t>
   </si>
   <si>
-    <t>60.63%</t>
+    <t>60.65%</t>
   </si>
   <si>
     <t>22R01A05L5</t>
@@ -2903,6 +2903,24 @@
     <t>18.15%</t>
   </si>
   <si>
+    <t>22R01A0409</t>
+  </si>
+  <si>
+    <t>Ramana333</t>
+  </si>
+  <si>
+    <t>22r01awyry</t>
+  </si>
+  <si>
+    <t>22r01a409</t>
+  </si>
+  <si>
+    <t>22r01a0409</t>
+  </si>
+  <si>
+    <t>17.98%</t>
+  </si>
+  <si>
     <t>22R01A6662</t>
   </si>
   <si>
@@ -2969,24 +2987,6 @@
     <t>17.07%</t>
   </si>
   <si>
-    <t>22R01A0409</t>
-  </si>
-  <si>
-    <t>Ramana333</t>
-  </si>
-  <si>
-    <t>22r01awyry</t>
-  </si>
-  <si>
-    <t>22r01a409</t>
-  </si>
-  <si>
-    <t>22r01a0409</t>
-  </si>
-  <si>
-    <t>16.99%</t>
-  </si>
-  <si>
     <t>22R01A67A5</t>
   </si>
   <si>
@@ -4007,7 +4007,7 @@
     <t>a22r01a66a2</t>
   </si>
   <si>
-    <t>11.05%</t>
+    <t>11.1%</t>
   </si>
   <si>
     <t>22R01A73C3</t>
@@ -10573,7 +10573,7 @@
         <v>166.0</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>95.0</v>
+        <v>97.0</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>31</v>
@@ -19056,7 +19056,7 @@
         <v>964</v>
       </c>
       <c r="D198" s="2" t="n">
-        <v>354.0</v>
+        <v>0.0</v>
       </c>
       <c r="E198" s="2" t="s">
         <v>965</v>
@@ -19065,25 +19065,25 @@
         <v>0.0</v>
       </c>
       <c r="G198" s="2" t="n">
-        <v>0.0</v>
+        <v>62.0</v>
       </c>
       <c r="H198" s="2" t="s">
         <v>966</v>
       </c>
       <c r="I198" s="2" t="n">
-        <v>0.0</v>
+        <v>1411.0</v>
       </c>
       <c r="J198" s="2" t="s">
+        <v>964</v>
+      </c>
+      <c r="K198" s="2" t="n">
+        <v>998.0</v>
+      </c>
+      <c r="L198" s="2" t="s">
         <v>967</v>
       </c>
-      <c r="K198" s="2" t="n">
-        <v>1351.0</v>
-      </c>
-      <c r="L198" s="2" t="s">
-        <v>964</v>
-      </c>
       <c r="M198" s="2" t="n">
-        <v>0.0</v>
+        <v>47.0</v>
       </c>
       <c r="N198" s="2" t="s">
         <v>968</v>
@@ -19100,37 +19100,37 @@
         <v>970</v>
       </c>
       <c r="D199" s="2" t="n">
-        <v>344.0</v>
+        <v>354.0</v>
       </c>
       <c r="E199" s="2" t="s">
+        <v>971</v>
+      </c>
+      <c r="F199" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G199" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H199" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="I199" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J199" s="2" t="s">
+        <v>973</v>
+      </c>
+      <c r="K199" s="2" t="n">
+        <v>1351.0</v>
+      </c>
+      <c r="L199" s="2" t="s">
         <v>970</v>
       </c>
-      <c r="F199" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G199" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H199" s="2" t="s">
-        <v>970</v>
-      </c>
-      <c r="I199" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J199" s="2" t="s">
-        <v>971</v>
-      </c>
-      <c r="K199" s="2" t="n">
-        <v>1021.0</v>
-      </c>
-      <c r="L199" s="2" t="s">
-        <v>972</v>
-      </c>
       <c r="M199" s="2" t="n">
-        <v>35.0</v>
+        <v>0.0</v>
       </c>
       <c r="N199" s="2" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
     </row>
     <row r="200">
@@ -19138,13 +19138,13 @@
         <v>199.0</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="D200" s="2" t="n">
-        <v>359.0</v>
+        <v>344.0</v>
       </c>
       <c r="E200" s="2" t="s">
         <v>976</v>
@@ -19165,16 +19165,16 @@
         <v>977</v>
       </c>
       <c r="K200" s="2" t="n">
-        <v>1218.0</v>
+        <v>1021.0</v>
       </c>
       <c r="L200" s="2" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="M200" s="2" t="n">
-        <v>0.0</v>
+        <v>35.0</v>
       </c>
       <c r="N200" s="2" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
     </row>
     <row r="201">
@@ -19182,16 +19182,16 @@
         <v>200.0</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>270</v>
+        <v>981</v>
       </c>
       <c r="D201" s="2" t="n">
-        <v>0.0</v>
+        <v>359.0</v>
       </c>
       <c r="E201" s="2" t="s">
-        <v>979</v>
+        <v>982</v>
       </c>
       <c r="F201" s="2" t="n">
         <v>0.0</v>
@@ -19200,25 +19200,25 @@
         <v>0.0</v>
       </c>
       <c r="H201" s="2" t="s">
-        <v>979</v>
+        <v>982</v>
       </c>
       <c r="I201" s="2" t="n">
-        <v>1485.0</v>
+        <v>0.0</v>
       </c>
       <c r="J201" s="2" t="s">
-        <v>979</v>
+        <v>983</v>
       </c>
       <c r="K201" s="2" t="n">
-        <v>0.0</v>
+        <v>1218.0</v>
       </c>
       <c r="L201" s="2" t="s">
-        <v>979</v>
+        <v>982</v>
       </c>
       <c r="M201" s="2" t="n">
-        <v>160.0</v>
+        <v>0.0</v>
       </c>
       <c r="N201" s="2" t="s">
-        <v>980</v>
+        <v>984</v>
       </c>
     </row>
     <row r="202">
@@ -19226,43 +19226,43 @@
         <v>201.0</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>981</v>
+        <v>985</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>982</v>
+        <v>270</v>
       </c>
       <c r="D202" s="2" t="n">
-        <v>388.0</v>
+        <v>0.0</v>
       </c>
       <c r="E202" s="2" t="s">
-        <v>982</v>
+        <v>985</v>
       </c>
       <c r="F202" s="2" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="G202" s="2" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="H202" s="2" t="s">
-        <v>982</v>
+        <v>985</v>
       </c>
       <c r="I202" s="2" t="n">
-        <v>0.0</v>
+        <v>1485.0</v>
       </c>
       <c r="J202" s="2" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="K202" s="2" t="n">
-        <v>888.0</v>
+        <v>0.0</v>
       </c>
       <c r="L202" s="2" t="s">
-        <v>981</v>
+        <v>985</v>
       </c>
       <c r="M202" s="2" t="n">
-        <v>0.0</v>
+        <v>160.0</v>
       </c>
       <c r="N202" s="2" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
     </row>
     <row r="203">
@@ -19270,40 +19270,40 @@
         <v>202.0</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="D203" s="2" t="n">
-        <v>0.0</v>
+        <v>388.0</v>
       </c>
       <c r="E203" s="2" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="F203" s="2" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="G203" s="2" t="n">
-        <v>62.0</v>
+        <v>2.0</v>
       </c>
       <c r="H203" s="2" t="s">
         <v>988</v>
       </c>
       <c r="I203" s="2" t="n">
-        <v>1411.0</v>
+        <v>0.0</v>
       </c>
       <c r="J203" s="2" t="s">
-        <v>986</v>
+        <v>989</v>
       </c>
       <c r="K203" s="2" t="n">
-        <v>998.0</v>
+        <v>888.0</v>
       </c>
       <c r="L203" s="2" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="M203" s="2" t="n">
-        <v>27.0</v>
+        <v>0.0</v>
       </c>
       <c r="N203" s="2" t="s">
         <v>990</v>
@@ -22339,7 +22339,7 @@
         <v>1328</v>
       </c>
       <c r="M272" s="2" t="n">
-        <v>103.0</v>
+        <v>104.0</v>
       </c>
       <c r="N272" s="2" t="s">
         <v>1331</v>

</xml_diff>

<commit_message>
Add generated leaderboard data - 2024-05-25T19:18:08
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
@@ -101,7 +101,7 @@
     <t>rohithgoje21</t>
   </si>
   <si>
-    <t>63.2%</t>
+    <t>63.22%</t>
   </si>
   <si>
     <t>22R01A0554</t>
@@ -113,7 +113,7 @@
     <t>sellilavanya</t>
   </si>
   <si>
-    <t>60.65%</t>
+    <t>60.69%</t>
   </si>
   <si>
     <t>22R01A05L5</t>
@@ -191,7 +191,7 @@
     <t>22r01a05l1</t>
   </si>
   <si>
-    <t>52.8%</t>
+    <t>52.81%</t>
   </si>
   <si>
     <t>22R01A66D5</t>
@@ -4007,7 +4007,7 @@
     <t>a22r01a66a2</t>
   </si>
   <si>
-    <t>11.1%</t>
+    <t>11.18%</t>
   </si>
   <si>
     <t>22R01A73C3</t>
@@ -10529,7 +10529,7 @@
         <v>244.0</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>175.0</v>
+        <v>177.0</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>28</v>
@@ -10573,7 +10573,7 @@
         <v>166.0</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>97.0</v>
+        <v>101.0</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>31</v>
@@ -10793,7 +10793,7 @@
         <v>80.0</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>208.0</v>
+        <v>210.0</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>56</v>
@@ -22321,7 +22321,7 @@
         <v>0.0</v>
       </c>
       <c r="G272" s="2" t="n">
-        <v>19.0</v>
+        <v>27.0</v>
       </c>
       <c r="H272" s="2" t="s">
         <v>1328</v>

</xml_diff>

<commit_message>
Add generated leaderboard data - 2024-05-31T03:43:48
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
@@ -48111,7 +48111,7 @@
         <v>80.0</v>
       </c>
       <c r="G888" s="2" t="n">
-        <v>210.0</v>
+        <v>212.0</v>
       </c>
       <c r="H888" s="2" t="s">
         <v>2344</v>
@@ -48859,7 +48859,7 @@
         <v>114.0</v>
       </c>
       <c r="G905" s="2" t="n">
-        <v>106.0</v>
+        <v>108.0</v>
       </c>
       <c r="H905" s="2" t="s">
         <v>2396</v>

</xml_diff>

<commit_message>
Add generated leaderboard data - 2024-06-01T19:19:40
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
@@ -101,7 +101,7 @@
     <t>rohithgoje21</t>
   </si>
   <si>
-    <t>63.66%</t>
+    <t>63.68%</t>
   </si>
   <si>
     <t>22R01A66D5</t>
@@ -125,7 +125,7 @@
     <t>sellilavanya</t>
   </si>
   <si>
-    <t>61.35%</t>
+    <t>61.38%</t>
   </si>
   <si>
     <t>22R01A05L5</t>
@@ -7094,6 +7094,18 @@
     <t>vennela_414</t>
   </si>
   <si>
+    <t>22R01A6790</t>
+  </si>
+  <si>
+    <t>Glory1510</t>
+  </si>
+  <si>
+    <t>Glory</t>
+  </si>
+  <si>
+    <t>glorysucharitha1</t>
+  </si>
+  <si>
     <t>22R01A0475</t>
   </si>
   <si>
@@ -7149,18 +7161,6 @@
   </si>
   <si>
     <t>23r05a6714</t>
-  </si>
-  <si>
-    <t>22R01A6790</t>
-  </si>
-  <si>
-    <t>Glory1510</t>
-  </si>
-  <si>
-    <t>Glory</t>
-  </si>
-  <si>
-    <t>glorysucharitha1</t>
   </si>
   <si>
     <t>22R01A67J7</t>
@@ -10553,7 +10553,7 @@
         <v>254.0</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>183.0</v>
+        <v>185.0</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>28</v>
@@ -10641,7 +10641,7 @@
         <v>176.0</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>111.0</v>
+        <v>114.0</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>35</v>
@@ -32497,13 +32497,13 @@
         <v>2360</v>
       </c>
       <c r="C503" s="2" t="s">
-        <v>193</v>
+        <v>2361</v>
       </c>
       <c r="D503" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E503" s="2" t="s">
-        <v>2361</v>
+        <v>2362</v>
       </c>
       <c r="F503" s="2" t="n">
         <v>0.0</v>
@@ -32512,7 +32512,7 @@
         <v>0.0</v>
       </c>
       <c r="H503" s="2" t="s">
-        <v>2361</v>
+        <v>2362</v>
       </c>
       <c r="I503" s="2" t="n">
         <v>0.0</v>
@@ -32524,7 +32524,7 @@
         <v>0.0</v>
       </c>
       <c r="L503" s="2" t="s">
-        <v>2361</v>
+        <v>2363</v>
       </c>
       <c r="M503" s="2" t="n">
         <v>6.0</v>
@@ -32538,10 +32538,10 @@
         <v>503.0</v>
       </c>
       <c r="B504" s="2" t="s">
-        <v>2363</v>
+        <v>2364</v>
       </c>
       <c r="C504" s="2" t="s">
-        <v>2364</v>
+        <v>193</v>
       </c>
       <c r="D504" s="2" t="n">
         <v>0.0</v>
@@ -32556,7 +32556,7 @@
         <v>0.0</v>
       </c>
       <c r="H504" s="2" t="s">
-        <v>2364</v>
+        <v>2365</v>
       </c>
       <c r="I504" s="2" t="n">
         <v>0.0</v>
@@ -32568,7 +32568,7 @@
         <v>0.0</v>
       </c>
       <c r="L504" s="2" t="s">
-        <v>2367</v>
+        <v>2365</v>
       </c>
       <c r="M504" s="2" t="n">
         <v>6.0</v>
@@ -32582,10 +32582,10 @@
         <v>504.0</v>
       </c>
       <c r="B505" s="2" t="s">
+        <v>2367</v>
+      </c>
+      <c r="C505" s="2" t="s">
         <v>2368</v>
-      </c>
-      <c r="C505" s="2" t="s">
-        <v>2369</v>
       </c>
       <c r="D505" s="2" t="n">
         <v>0.0</v>
@@ -32600,25 +32600,25 @@
         <v>0.0</v>
       </c>
       <c r="H505" s="2" t="s">
-        <v>2369</v>
+        <v>2368</v>
       </c>
       <c r="I505" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="J505" s="2" t="s">
-        <v>2369</v>
+        <v>2370</v>
       </c>
       <c r="K505" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="L505" s="2" t="s">
-        <v>2369</v>
+        <v>2371</v>
       </c>
       <c r="M505" s="2" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="N505" s="2" t="s">
-        <v>2370</v>
+        <v>2353</v>
       </c>
     </row>
     <row r="506">
@@ -32626,16 +32626,16 @@
         <v>505.0</v>
       </c>
       <c r="B506" s="2" t="s">
-        <v>2371</v>
+        <v>2372</v>
       </c>
       <c r="C506" s="2" t="s">
-        <v>2371</v>
+        <v>2373</v>
       </c>
       <c r="D506" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E506" s="2" t="s">
-        <v>2372</v>
+        <v>2373</v>
       </c>
       <c r="F506" s="2" t="n">
         <v>0.0</v>
@@ -32650,19 +32650,19 @@
         <v>0.0</v>
       </c>
       <c r="J506" s="2" t="s">
-        <v>193</v>
+        <v>2373</v>
       </c>
       <c r="K506" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="L506" s="2" t="s">
+        <v>2373</v>
+      </c>
+      <c r="M506" s="2" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="N506" s="2" t="s">
         <v>2374</v>
-      </c>
-      <c r="M506" s="2" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="N506" s="2" t="s">
-        <v>2375</v>
       </c>
     </row>
     <row r="507">
@@ -32670,25 +32670,25 @@
         <v>506.0</v>
       </c>
       <c r="B507" s="2" t="s">
+        <v>2375</v>
+      </c>
+      <c r="C507" s="2" t="s">
+        <v>2375</v>
+      </c>
+      <c r="D507" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E507" s="2" t="s">
         <v>2376</v>
       </c>
-      <c r="C507" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="D507" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E507" s="2" t="s">
+      <c r="F507" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G507" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H507" s="2" t="s">
         <v>2377</v>
-      </c>
-      <c r="F507" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G507" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H507" s="2" t="s">
-        <v>193</v>
       </c>
       <c r="I507" s="2" t="n">
         <v>0.0</v>
@@ -32706,7 +32706,7 @@
         <v>4.0</v>
       </c>
       <c r="N507" s="2" t="s">
-        <v>2375</v>
+        <v>2379</v>
       </c>
     </row>
     <row r="508">
@@ -32714,10 +32714,10 @@
         <v>507.0</v>
       </c>
       <c r="B508" s="2" t="s">
-        <v>2379</v>
+        <v>2380</v>
       </c>
       <c r="C508" s="2" t="s">
-        <v>2380</v>
+        <v>193</v>
       </c>
       <c r="D508" s="2" t="n">
         <v>0.0</v>
@@ -32732,13 +32732,13 @@
         <v>0.0</v>
       </c>
       <c r="H508" s="2" t="s">
-        <v>2381</v>
+        <v>193</v>
       </c>
       <c r="I508" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="J508" s="2" t="s">
-        <v>2381</v>
+        <v>193</v>
       </c>
       <c r="K508" s="2" t="n">
         <v>0.0</v>
@@ -32750,7 +32750,7 @@
         <v>4.0</v>
       </c>
       <c r="N508" s="2" t="s">
-        <v>2375</v>
+        <v>2379</v>
       </c>
     </row>
     <row r="509">

</xml_diff>

<commit_message>
Add generated leaderboard data - 2024-06-11T19:19:43
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
@@ -125,7 +125,7 @@
     <t>sellilavanya</t>
   </si>
   <si>
-    <t>59.47</t>
+    <t>59.51</t>
   </si>
   <si>
     <t>22R01A0531</t>
@@ -419,7 +419,7 @@
     <t>koushikpatel</t>
   </si>
   <si>
-    <t>40.96</t>
+    <t>41.16</t>
   </si>
   <si>
     <t>22R01A04C3</t>
@@ -1244,6 +1244,21 @@
     <t>32.77</t>
   </si>
   <si>
+    <t>22R01A0517</t>
+  </si>
+  <si>
+    <t>akshaya_23</t>
+  </si>
+  <si>
+    <t>22r01a0517</t>
+  </si>
+  <si>
+    <t>akshuspoorthi</t>
+  </si>
+  <si>
+    <t>32.68</t>
+  </si>
+  <si>
     <t>22R01A6673</t>
   </si>
   <si>
@@ -1401,21 +1416,6 @@
   </si>
   <si>
     <t>31.24</t>
-  </si>
-  <si>
-    <t>22R01A0517</t>
-  </si>
-  <si>
-    <t>akshaya_23</t>
-  </si>
-  <si>
-    <t>22r01a0517</t>
-  </si>
-  <si>
-    <t>akshuspoorthi</t>
-  </si>
-  <si>
-    <t>31.21</t>
   </si>
   <si>
     <t>22R01A6780</t>
@@ -10761,7 +10761,7 @@
         <v>186.0</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>132.0</v>
+        <v>136.0</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>35</v>
@@ -11641,7 +11641,7 @@
         <v>0.0</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>37.0</v>
+        <v>57.0</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>133</v>
@@ -14184,34 +14184,34 @@
         <v>411</v>
       </c>
       <c r="D84" s="2" t="n">
-        <v>382.0</v>
+        <v>604.0</v>
       </c>
       <c r="E84" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="F84" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G84" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H84" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="F84" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G84" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H84" s="2" t="s">
+      <c r="I84" s="2" t="n">
+        <v>1380.0</v>
+      </c>
+      <c r="J84" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="I84" s="2" t="n">
-        <v>1412.0</v>
-      </c>
-      <c r="J84" s="2" t="s">
-        <v>411</v>
-      </c>
       <c r="K84" s="2" t="n">
-        <v>931.0</v>
+        <v>1122.0</v>
       </c>
       <c r="L84" s="2" t="s">
         <v>411</v>
       </c>
       <c r="M84" s="2" t="n">
-        <v>165.0</v>
+        <v>33.0</v>
       </c>
       <c r="N84" s="2" t="s">
         <v>414</v>
@@ -14228,10 +14228,10 @@
         <v>416</v>
       </c>
       <c r="D85" s="2" t="n">
-        <v>639.0</v>
+        <v>382.0</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F85" s="2" t="n">
         <v>0.0</v>
@@ -14240,25 +14240,25 @@
         <v>0.0</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="I85" s="2" t="n">
-        <v>1418.0</v>
+        <v>1412.0</v>
       </c>
       <c r="J85" s="2" t="s">
         <v>416</v>
       </c>
       <c r="K85" s="2" t="n">
-        <v>1171.0</v>
+        <v>931.0</v>
       </c>
       <c r="L85" s="2" t="s">
         <v>416</v>
       </c>
       <c r="M85" s="2" t="n">
-        <v>0.0</v>
+        <v>165.0</v>
       </c>
       <c r="N85" s="2" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="86">
@@ -14266,16 +14266,16 @@
         <v>85.0</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="D86" s="2" t="n">
-        <v>577.0</v>
+        <v>639.0</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>206</v>
+        <v>421</v>
       </c>
       <c r="F86" s="2" t="n">
         <v>0.0</v>
@@ -14284,25 +14284,25 @@
         <v>0.0</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="I86" s="2" t="n">
-        <v>1595.0</v>
+        <v>1418.0</v>
       </c>
       <c r="J86" s="2" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="K86" s="2" t="n">
-        <v>1231.0</v>
+        <v>1171.0</v>
       </c>
       <c r="L86" s="2" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="M86" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="N86" s="2" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="87">
@@ -14310,43 +14310,43 @@
         <v>86.0</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="D87" s="2" t="n">
-        <v>579.0</v>
+        <v>577.0</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>422</v>
+        <v>206</v>
       </c>
       <c r="F87" s="2" t="n">
-        <v>17.0</v>
+        <v>0.0</v>
       </c>
       <c r="G87" s="2" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="I87" s="2" t="n">
-        <v>1151.0</v>
+        <v>1595.0</v>
       </c>
       <c r="J87" s="2" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="K87" s="2" t="n">
-        <v>1046.0</v>
+        <v>1231.0</v>
       </c>
       <c r="L87" s="2" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="M87" s="2" t="n">
-        <v>35.0</v>
+        <v>0.0</v>
       </c>
       <c r="N87" s="2" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="88">
@@ -14354,40 +14354,40 @@
         <v>87.0</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="D88" s="2" t="n">
-        <v>783.0</v>
+        <v>579.0</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="F88" s="2" t="n">
-        <v>0.0</v>
+        <v>17.0</v>
       </c>
       <c r="G88" s="2" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="H88" s="2" t="s">
         <v>427</v>
       </c>
       <c r="I88" s="2" t="n">
-        <v>1451.0</v>
+        <v>1151.0</v>
       </c>
       <c r="J88" s="2" t="s">
         <v>428</v>
       </c>
       <c r="K88" s="2" t="n">
-        <v>504.0</v>
+        <v>1046.0</v>
       </c>
       <c r="L88" s="2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="M88" s="2" t="n">
-        <v>2.0</v>
+        <v>35.0</v>
       </c>
       <c r="N88" s="2" t="s">
         <v>429</v>
@@ -14401,10 +14401,10 @@
         <v>430</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D89" s="2" t="n">
-        <v>573.0</v>
+        <v>783.0</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>431</v>
@@ -14413,28 +14413,28 @@
         <v>0.0</v>
       </c>
       <c r="G89" s="2" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="I89" s="2" t="n">
-        <v>1474.0</v>
+        <v>1451.0</v>
       </c>
       <c r="J89" s="2" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="K89" s="2" t="n">
-        <v>1242.0</v>
+        <v>504.0</v>
       </c>
       <c r="L89" s="2" t="s">
         <v>431</v>
       </c>
       <c r="M89" s="2" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="N89" s="2" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="90">
@@ -14442,43 +14442,43 @@
         <v>89.0</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>435</v>
       </c>
       <c r="D90" s="2" t="n">
-        <v>585.0</v>
+        <v>573.0</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>206</v>
+        <v>436</v>
       </c>
       <c r="F90" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="G90" s="2" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="I90" s="2" t="n">
-        <v>1364.0</v>
+        <v>1474.0</v>
       </c>
       <c r="J90" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="K90" s="2" t="n">
+        <v>1242.0</v>
+      </c>
+      <c r="L90" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="K90" s="2" t="n">
-        <v>1065.0</v>
-      </c>
-      <c r="L90" s="2" t="s">
-        <v>435</v>
-      </c>
       <c r="M90" s="2" t="n">
-        <v>35.0</v>
+        <v>5.0</v>
       </c>
       <c r="N90" s="2" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="91">
@@ -14486,40 +14486,40 @@
         <v>90.0</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="D91" s="2" t="n">
-        <v>588.0</v>
+        <v>585.0</v>
       </c>
       <c r="E91" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F91" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G91" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H91" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="F91" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G91" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H91" s="2" t="s">
-        <v>439</v>
-      </c>
       <c r="I91" s="2" t="n">
-        <v>1320.0</v>
+        <v>1364.0</v>
       </c>
       <c r="J91" s="2" t="s">
         <v>441</v>
       </c>
       <c r="K91" s="2" t="n">
-        <v>1062.0</v>
+        <v>1065.0</v>
       </c>
       <c r="L91" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="M91" s="2" t="n">
-        <v>32.0</v>
+        <v>35.0</v>
       </c>
       <c r="N91" s="2" t="s">
         <v>442</v>
@@ -14536,7 +14536,7 @@
         <v>444</v>
       </c>
       <c r="D92" s="2" t="n">
-        <v>572.0</v>
+        <v>588.0</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>445</v>
@@ -14548,25 +14548,25 @@
         <v>0.0</v>
       </c>
       <c r="H92" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="I92" s="2" t="n">
+        <v>1320.0</v>
+      </c>
+      <c r="J92" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="I92" s="2" t="n">
-        <v>1271.0</v>
-      </c>
-      <c r="J92" s="2" t="s">
+      <c r="K92" s="2" t="n">
+        <v>1062.0</v>
+      </c>
+      <c r="L92" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="M92" s="2" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="N92" s="2" t="s">
         <v>447</v>
-      </c>
-      <c r="K92" s="2" t="n">
-        <v>1268.0</v>
-      </c>
-      <c r="L92" s="2" t="s">
-        <v>448</v>
-      </c>
-      <c r="M92" s="2" t="n">
-        <v>16.0</v>
-      </c>
-      <c r="N92" s="2" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="93">
@@ -14574,43 +14574,43 @@
         <v>92.0</v>
       </c>
       <c r="B93" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="D93" s="2" t="n">
+        <v>572.0</v>
+      </c>
+      <c r="E93" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="F93" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G93" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H93" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="D93" s="2" t="n">
-        <v>782.0</v>
-      </c>
-      <c r="E93" s="2" t="s">
+      <c r="I93" s="2" t="n">
+        <v>1271.0</v>
+      </c>
+      <c r="J93" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="F93" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G93" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H93" s="2" t="s">
+      <c r="K93" s="2" t="n">
+        <v>1268.0</v>
+      </c>
+      <c r="L93" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="I93" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J93" s="2" t="s">
+      <c r="M93" s="2" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="N93" s="2" t="s">
         <v>454</v>
-      </c>
-      <c r="K93" s="2" t="n">
-        <v>421.0</v>
-      </c>
-      <c r="L93" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="M93" s="2" t="n">
-        <v>182.0</v>
-      </c>
-      <c r="N93" s="2" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="94">
@@ -14618,43 +14618,43 @@
         <v>93.0</v>
       </c>
       <c r="B94" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="D94" s="2" t="n">
+        <v>782.0</v>
+      </c>
+      <c r="E94" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="F94" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G94" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H94" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="D94" s="2" t="n">
-        <v>816.0</v>
-      </c>
-      <c r="E94" s="2" t="s">
+      <c r="I94" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J94" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="F94" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G94" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H94" s="2" t="s">
+      <c r="K94" s="2" t="n">
+        <v>421.0</v>
+      </c>
+      <c r="L94" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="I94" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J94" s="2" t="s">
+      <c r="M94" s="2" t="n">
+        <v>182.0</v>
+      </c>
+      <c r="N94" s="2" t="s">
         <v>461</v>
-      </c>
-      <c r="K94" s="2" t="n">
-        <v>864.0</v>
-      </c>
-      <c r="L94" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="M94" s="2" t="n">
-        <v>103.0</v>
-      </c>
-      <c r="N94" s="2" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="95">
@@ -14662,13 +14662,13 @@
         <v>94.0</v>
       </c>
       <c r="B95" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="C95" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="C95" s="2" t="s">
-        <v>464</v>
-      </c>
       <c r="D95" s="2" t="n">
-        <v>604.0</v>
+        <v>816.0</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>464</v>
@@ -14683,19 +14683,19 @@
         <v>465</v>
       </c>
       <c r="I95" s="2" t="n">
-        <v>1380.0</v>
+        <v>0.0</v>
       </c>
       <c r="J95" s="2" t="s">
         <v>466</v>
       </c>
       <c r="K95" s="2" t="n">
-        <v>1122.0</v>
+        <v>864.0</v>
       </c>
       <c r="L95" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="M95" s="2" t="n">
-        <v>3.0</v>
+        <v>103.0</v>
       </c>
       <c r="N95" s="2" t="s">
         <v>467</v>

</xml_diff>

<commit_message>
Add generated leaderboard data - 2024-06-15T19:18:35
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
@@ -125,7 +125,7 @@
     <t>sellilavanya</t>
   </si>
   <si>
-    <t>59.25</t>
+    <t>59.29</t>
   </si>
   <si>
     <t>22R01A0531</t>
@@ -10815,7 +10815,7 @@
         <v>186.0</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>140.0</v>
+        <v>144.0</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Add generated leaderboard data - 2024-06-20T19:19:33
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
@@ -158,7 +158,7 @@
     <t>KIREET_5L5</t>
   </si>
   <si>
-    <t>55.41</t>
+    <t>55.51</t>
   </si>
   <si>
     <t>22R01A05C9</t>
@@ -10903,7 +10903,7 @@
         <v>60.0</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>296.0</v>
+        <v>306.0</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Add generated leaderboard data - 2024-06-30T19:19:16
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
@@ -140,7 +140,7 @@
     <t>sellilavanya</t>
   </si>
   <si>
-    <t>59.09</t>
+    <t>59.11</t>
   </si>
   <si>
     <t>22R01A05L5</t>
@@ -161,7 +161,7 @@
     <t>KIREET_5L5</t>
   </si>
   <si>
-    <t>55.35</t>
+    <t>55.4</t>
   </si>
   <si>
     <t>22R01A05C9</t>
@@ -3860,7 +3860,7 @@
     <t>vanisathvika</t>
   </si>
   <si>
-    <t>15.64</t>
+    <t>15.65</t>
   </si>
   <si>
     <t>22R01A0456</t>
@@ -10859,7 +10859,7 @@
         <v>186.0</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>156.0</v>
+        <v>158.0</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>40</v>
@@ -10903,7 +10903,7 @@
         <v>60.0</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>312.0</v>
+        <v>317.0</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>46</v>
@@ -22035,7 +22035,7 @@
         <v>0.0</v>
       </c>
       <c r="G261" s="2" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H261" s="2" t="s">
         <v>1280</v>

</xml_diff>

<commit_message>
Add generated leaderboard data - 2024-07-04T19:21:30
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
@@ -71,7 +71,7 @@
     <t>shivakrishnamur1</t>
   </si>
   <si>
-    <t>66.0</t>
+    <t>66.03</t>
   </si>
   <si>
     <t>22R01A7339</t>
@@ -797,6 +797,36 @@
     <t>36.33</t>
   </si>
   <si>
+    <t>22R01A05N5</t>
+  </si>
+  <si>
+    <t>navaneethmahar</t>
+  </si>
+  <si>
+    <t>22r01a05n5</t>
+  </si>
+  <si>
+    <t>navaneethmahara</t>
+  </si>
+  <si>
+    <t>navaneethmahara1</t>
+  </si>
+  <si>
+    <t>35.99</t>
+  </si>
+  <si>
+    <t>23R05A0525</t>
+  </si>
+  <si>
+    <t>23r05a0525</t>
+  </si>
+  <si>
+    <t>23r05a1nal</t>
+  </si>
+  <si>
+    <t>cmr23r05a0525</t>
+  </si>
+  <si>
     <t>22R01A0505</t>
   </si>
   <si>
@@ -806,37 +836,7 @@
     <t>eshu5886</t>
   </si>
   <si>
-    <t>36.14</t>
-  </si>
-  <si>
-    <t>22R01A05N5</t>
-  </si>
-  <si>
-    <t>navaneethmahar</t>
-  </si>
-  <si>
-    <t>22r01a05n5</t>
-  </si>
-  <si>
-    <t>navaneethmahara</t>
-  </si>
-  <si>
-    <t>navaneethmahara1</t>
-  </si>
-  <si>
-    <t>35.99</t>
-  </si>
-  <si>
-    <t>23R05A0525</t>
-  </si>
-  <si>
-    <t>23r05a0525</t>
-  </si>
-  <si>
-    <t>23r05a1nal</t>
-  </si>
-  <si>
-    <t>cmr23r05a0525</t>
+    <t>35.96</t>
   </si>
   <si>
     <t>22R01A05B0</t>
@@ -848,9 +848,6 @@
     <t>22r01a05b0</t>
   </si>
   <si>
-    <t>35.96</t>
-  </si>
-  <si>
     <t>23R05A6705</t>
   </si>
   <si>
@@ -1067,6 +1064,18 @@
     <t>34.17</t>
   </si>
   <si>
+    <t>23R05A0501</t>
+  </si>
+  <si>
+    <t>sreemahi</t>
+  </si>
+  <si>
+    <t>23r05a0501</t>
+  </si>
+  <si>
+    <t>34.04</t>
+  </si>
+  <si>
     <t>22R01A6235</t>
   </si>
   <si>
@@ -1124,30 +1133,21 @@
     <t>33.68</t>
   </si>
   <si>
-    <t>23R05A0501</t>
-  </si>
-  <si>
-    <t>sreemahi</t>
-  </si>
-  <si>
-    <t>23r05a0501</t>
+    <t>22R01A67D0</t>
+  </si>
+  <si>
+    <t>sujith09</t>
+  </si>
+  <si>
+    <t>sujith90</t>
+  </si>
+  <si>
+    <t>22r01a67d0</t>
   </si>
   <si>
     <t>33.67</t>
   </si>
   <si>
-    <t>22R01A67D0</t>
-  </si>
-  <si>
-    <t>sujith09</t>
-  </si>
-  <si>
-    <t>sujith90</t>
-  </si>
-  <si>
-    <t>22r01a67d0</t>
-  </si>
-  <si>
     <t>22R01A05R2</t>
   </si>
   <si>
@@ -2225,7 +2225,7 @@
     <t>cse_22r01a0559</t>
   </si>
   <si>
-    <t>26.18</t>
+    <t>26.14</t>
   </si>
   <si>
     <t>23R05A0512</t>
@@ -3593,6 +3593,75 @@
     <t>16.29</t>
   </si>
   <si>
+    <t>22R01A66J8</t>
+  </si>
+  <si>
+    <t>pooj_v227</t>
+  </si>
+  <si>
+    <t>poojav_66j8</t>
+  </si>
+  <si>
+    <t>poojav_227</t>
+  </si>
+  <si>
+    <t>22r01a66j8</t>
+  </si>
+  <si>
+    <t>16.21</t>
+  </si>
+  <si>
+    <t>22R01A6251</t>
+  </si>
+  <si>
+    <t>nerella_vaishnavi</t>
+  </si>
+  <si>
+    <t>nerella_15</t>
+  </si>
+  <si>
+    <t>22r01a6251</t>
+  </si>
+  <si>
+    <t>16.18</t>
+  </si>
+  <si>
+    <t>22R01A05C4</t>
+  </si>
+  <si>
+    <t>SanjayTalari</t>
+  </si>
+  <si>
+    <t>16.16</t>
+  </si>
+  <si>
+    <t>22R01A6699</t>
+  </si>
+  <si>
+    <t>22r01a6699</t>
+  </si>
+  <si>
+    <t>manasanipavan</t>
+  </si>
+  <si>
+    <t>16.14</t>
+  </si>
+  <si>
+    <t>22R01A05K9</t>
+  </si>
+  <si>
+    <t>banothmohanms</t>
+  </si>
+  <si>
+    <t>mohan5k9</t>
+  </si>
+  <si>
+    <t>Mohan5k9</t>
+  </si>
+  <si>
+    <t>16.08</t>
+  </si>
+  <si>
     <t>22R01A67J9</t>
   </si>
   <si>
@@ -3602,76 +3671,7 @@
     <t>mukesh_75</t>
   </si>
   <si>
-    <t>16.28</t>
-  </si>
-  <si>
-    <t>22R01A66J8</t>
-  </si>
-  <si>
-    <t>pooj_v227</t>
-  </si>
-  <si>
-    <t>poojav_66j8</t>
-  </si>
-  <si>
-    <t>poojav_227</t>
-  </si>
-  <si>
-    <t>22r01a66j8</t>
-  </si>
-  <si>
-    <t>16.21</t>
-  </si>
-  <si>
-    <t>22R01A6251</t>
-  </si>
-  <si>
-    <t>nerella_vaishnavi</t>
-  </si>
-  <si>
-    <t>nerella_15</t>
-  </si>
-  <si>
-    <t>22r01a6251</t>
-  </si>
-  <si>
-    <t>16.18</t>
-  </si>
-  <si>
-    <t>22R01A05C4</t>
-  </si>
-  <si>
-    <t>SanjayTalari</t>
-  </si>
-  <si>
-    <t>16.16</t>
-  </si>
-  <si>
-    <t>22R01A6699</t>
-  </si>
-  <si>
-    <t>22r01a6699</t>
-  </si>
-  <si>
-    <t>manasanipavan</t>
-  </si>
-  <si>
-    <t>16.14</t>
-  </si>
-  <si>
-    <t>22R01A05K9</t>
-  </si>
-  <si>
-    <t>banothmohanms</t>
-  </si>
-  <si>
-    <t>mohan5k9</t>
-  </si>
-  <si>
-    <t>Mohan5k9</t>
-  </si>
-  <si>
-    <t>16.08</t>
+    <t>16.02</t>
   </si>
   <si>
     <t>22R01A0581</t>
@@ -4802,6 +4802,15 @@
     <t>8.79</t>
   </si>
   <si>
+    <t>22R01A05L0</t>
+  </si>
+  <si>
+    <t>22r01a05l0</t>
+  </si>
+  <si>
+    <t>8.72</t>
+  </si>
+  <si>
     <t>22R01A0491</t>
   </si>
   <si>
@@ -4811,16 +4820,7 @@
     <t>Varsha_29</t>
   </si>
   <si>
-    <t>8.76</t>
-  </si>
-  <si>
-    <t>22R01A05L0</t>
-  </si>
-  <si>
-    <t>22r01a05l0</t>
-  </si>
-  <si>
-    <t>8.72</t>
+    <t>8.54</t>
   </si>
   <si>
     <t>23R05A0505</t>
@@ -10648,7 +10648,7 @@
         <v>60.0</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>68.0</v>
+        <v>71.0</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>14</v>
@@ -12883,37 +12883,37 @@
         <v>262</v>
       </c>
       <c r="D53" s="2" t="n">
-        <v>716.0</v>
+        <v>729.0</v>
       </c>
       <c r="E53" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="F53" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G53" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="I53" s="2" t="n">
+        <v>1404.0</v>
+      </c>
+      <c r="J53" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="F53" s="2" t="n">
-        <v>27.0</v>
-      </c>
-      <c r="G53" s="2" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="I53" s="2" t="n">
-        <v>1090.0</v>
-      </c>
-      <c r="J53" s="2" t="s">
-        <v>263</v>
-      </c>
       <c r="K53" s="2" t="n">
-        <v>1074.0</v>
+        <v>1228.0</v>
       </c>
       <c r="L53" s="2" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="M53" s="2" t="n">
-        <v>35.0</v>
+        <v>25.0</v>
       </c>
       <c r="N53" s="2" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="54">
@@ -12921,16 +12921,16 @@
         <v>53.0</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D54" s="2" t="n">
-        <v>729.0</v>
+        <v>726.0</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="F54" s="2" t="n">
         <v>0.0</v>
@@ -12942,22 +12942,22 @@
         <v>268</v>
       </c>
       <c r="I54" s="2" t="n">
-        <v>1404.0</v>
+        <v>1477.0</v>
       </c>
       <c r="J54" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="K54" s="2" t="n">
+        <v>1063.0</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="M54" s="2" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="N54" s="2" t="s">
         <v>266</v>
-      </c>
-      <c r="K54" s="2" t="n">
-        <v>1228.0</v>
-      </c>
-      <c r="L54" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="M54" s="2" t="n">
-        <v>25.0</v>
-      </c>
-      <c r="N54" s="2" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="55">
@@ -12971,37 +12971,37 @@
         <v>272</v>
       </c>
       <c r="D55" s="2" t="n">
-        <v>726.0</v>
+        <v>716.0</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F55" s="2" t="n">
-        <v>0.0</v>
+        <v>27.0</v>
       </c>
       <c r="G55" s="2" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>272</v>
       </c>
       <c r="I55" s="2" t="n">
-        <v>1477.0</v>
+        <v>1060.0</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K55" s="2" t="n">
-        <v>1063.0</v>
+        <v>1074.0</v>
       </c>
       <c r="L55" s="2" t="s">
         <v>272</v>
       </c>
       <c r="M55" s="2" t="n">
-        <v>40.0</v>
+        <v>35.0</v>
       </c>
       <c r="N55" s="2" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="56">
@@ -13045,7 +13045,7 @@
         <v>46.0</v>
       </c>
       <c r="N56" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="57">
@@ -13053,16 +13053,16 @@
         <v>56.0</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>280</v>
       </c>
       <c r="D57" s="2" t="n">
         <v>842.0</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F57" s="2" t="n">
         <v>0.0</v>
@@ -13071,25 +13071,25 @@
         <v>0.0</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I57" s="2" t="n">
         <v>1381.0</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K57" s="2" t="n">
         <v>980.0</v>
       </c>
       <c r="L57" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="M57" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="N57" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="58">
@@ -13097,16 +13097,16 @@
         <v>57.0</v>
       </c>
       <c r="B58" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>284</v>
       </c>
       <c r="D58" s="2" t="n">
         <v>715.0</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F58" s="2" t="n">
         <v>10.0</v>
@@ -13115,25 +13115,25 @@
         <v>2.0</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I58" s="2" t="n">
         <v>1422.0</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K58" s="2" t="n">
         <v>1255.0</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="M58" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="N58" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="59">
@@ -13141,16 +13141,16 @@
         <v>58.0</v>
       </c>
       <c r="B59" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>290</v>
       </c>
       <c r="D59" s="2" t="n">
         <v>769.0</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F59" s="2" t="n">
         <v>10.0</v>
@@ -13159,25 +13159,25 @@
         <v>0.0</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I59" s="2" t="n">
         <v>1315.0</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K59" s="2" t="n">
         <v>1099.0</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="M59" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="N59" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="60">
@@ -13185,43 +13185,43 @@
         <v>59.0</v>
       </c>
       <c r="B60" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>293</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>294</v>
       </c>
       <c r="D60" s="2" t="n">
         <v>745.0</v>
       </c>
       <c r="E60" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F60" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G60" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H60" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="F60" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G60" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H60" s="2" t="s">
+      <c r="I60" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J60" s="2" t="s">
         <v>296</v>
-      </c>
-      <c r="I60" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="J60" s="2" t="s">
-        <v>297</v>
       </c>
       <c r="K60" s="2" t="n">
         <v>1043.0</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="M60" s="2" t="n">
         <v>214.0</v>
       </c>
       <c r="N60" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="61">
@@ -13229,16 +13229,16 @@
         <v>60.0</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>299</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>300</v>
       </c>
       <c r="D61" s="2" t="n">
         <v>696.0</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F61" s="2" t="n">
         <v>0.0</v>
@@ -13247,25 +13247,25 @@
         <v>2.0</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I61" s="2" t="n">
         <v>1411.0</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K61" s="2" t="n">
         <v>1011.0</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="M61" s="2" t="n">
         <v>56.0</v>
       </c>
       <c r="N61" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="62">
@@ -13273,43 +13273,43 @@
         <v>61.0</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>303</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>304</v>
       </c>
       <c r="D62" s="2" t="n">
         <v>838.0</v>
       </c>
       <c r="E62" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="F62" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G62" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H62" s="2" t="s">
         <v>305</v>
-      </c>
-      <c r="F62" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G62" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>306</v>
       </c>
       <c r="I62" s="2" t="n">
         <v>1351.0</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="K62" s="2" t="n">
         <v>926.0</v>
       </c>
       <c r="L62" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="M62" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N62" s="2" t="s">
         <v>308</v>
-      </c>
-      <c r="M62" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N62" s="2" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="63">
@@ -13317,16 +13317,16 @@
         <v>62.0</v>
       </c>
       <c r="B63" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>310</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>311</v>
       </c>
       <c r="D63" s="2" t="n">
         <v>701.0</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F63" s="2" t="n">
         <v>8.0</v>
@@ -13335,25 +13335,25 @@
         <v>24.0</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I63" s="2" t="n">
         <v>1306.0</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K63" s="2" t="n">
         <v>1286.0</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M63" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="N63" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="64">
@@ -13361,16 +13361,16 @@
         <v>63.0</v>
       </c>
       <c r="B64" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>315</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>316</v>
       </c>
       <c r="D64" s="2" t="n">
         <v>838.0</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F64" s="2" t="n">
         <v>0.0</v>
@@ -13379,25 +13379,25 @@
         <v>1.0</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I64" s="2" t="n">
         <v>1304.0</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="K64" s="2" t="n">
         <v>794.0</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="M64" s="2" t="n">
         <v>20.0</v>
       </c>
       <c r="N64" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="65">
@@ -13405,16 +13405,16 @@
         <v>64.0</v>
       </c>
       <c r="B65" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>320</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>321</v>
       </c>
       <c r="D65" s="2" t="n">
         <v>754.0</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F65" s="2" t="n">
         <v>0.0</v>
@@ -13423,25 +13423,25 @@
         <v>0.0</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I65" s="2" t="n">
         <v>1412.0</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="K65" s="2" t="n">
         <v>1104.0</v>
       </c>
       <c r="L65" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="M65" s="2" t="n">
         <v>7.0</v>
       </c>
       <c r="N65" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="66">
@@ -13449,16 +13449,16 @@
         <v>65.0</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>324</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>325</v>
       </c>
       <c r="D66" s="2" t="n">
         <v>743.0</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F66" s="2" t="n">
         <v>0.0</v>
@@ -13467,25 +13467,25 @@
         <v>0.0</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I66" s="2" t="n">
         <v>1371.0</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="K66" s="2" t="n">
         <v>1030.0</v>
       </c>
       <c r="L66" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="M66" s="2" t="n">
         <v>25.0</v>
       </c>
       <c r="N66" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="67">
@@ -13493,16 +13493,16 @@
         <v>66.0</v>
       </c>
       <c r="B67" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>329</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>330</v>
       </c>
       <c r="D67" s="2" t="n">
         <v>733.0</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F67" s="2" t="n">
         <v>0.0</v>
@@ -13511,25 +13511,25 @@
         <v>0.0</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I67" s="2" t="n">
         <v>1389.0</v>
       </c>
       <c r="J67" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="K67" s="2" t="n">
         <v>1119.0</v>
       </c>
       <c r="L67" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="M67" s="2" t="n">
         <v>10.0</v>
       </c>
       <c r="N67" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="68">
@@ -13537,43 +13537,43 @@
         <v>67.0</v>
       </c>
       <c r="B68" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>334</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>335</v>
       </c>
       <c r="D68" s="2" t="n">
         <v>638.0</v>
       </c>
       <c r="E68" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="F68" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G68" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H68" s="2" t="s">
         <v>336</v>
-      </c>
-      <c r="F68" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G68" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H68" s="2" t="s">
-        <v>337</v>
       </c>
       <c r="I68" s="2" t="n">
         <v>1412.0</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="K68" s="2" t="n">
         <v>1238.0</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="M68" s="2" t="n">
         <v>40.0</v>
       </c>
       <c r="N68" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="69">
@@ -13581,10 +13581,10 @@
         <v>68.0</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>341</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>342</v>
       </c>
       <c r="D69" s="2" t="n">
         <v>763.0</v>
@@ -13599,25 +13599,25 @@
         <v>0.0</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I69" s="2" t="n">
         <v>1463.0</v>
       </c>
       <c r="J69" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K69" s="2" t="n">
         <v>911.0</v>
       </c>
       <c r="L69" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="M69" s="2" t="n">
         <v>6.0</v>
       </c>
       <c r="N69" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="70">
@@ -13625,43 +13625,43 @@
         <v>69.0</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C70" s="2" t="s">
         <v>345</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>346</v>
       </c>
       <c r="D70" s="2" t="n">
         <v>765.0</v>
       </c>
       <c r="E70" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="F70" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G70" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H70" s="2" t="s">
         <v>347</v>
-      </c>
-      <c r="F70" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G70" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H70" s="2" t="s">
-        <v>348</v>
       </c>
       <c r="I70" s="2" t="n">
         <v>1256.0</v>
       </c>
       <c r="J70" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="K70" s="2" t="n">
         <v>1130.0</v>
       </c>
       <c r="L70" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="M70" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N70" s="2" t="s">
         <v>349</v>
-      </c>
-      <c r="M70" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N70" s="2" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="71">
@@ -13669,43 +13669,43 @@
         <v>70.0</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="D71" s="2" t="n">
+        <v>660.0</v>
+      </c>
+      <c r="E71" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="D71" s="2" t="n">
-        <v>776.0</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>353</v>
-      </c>
       <c r="F71" s="2" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="G71" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="I71" s="2" t="n">
         <v>1412.0</v>
       </c>
       <c r="J71" s="2" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="K71" s="2" t="n">
-        <v>918.0</v>
+        <v>1202.0</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="M71" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="N71" s="2" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="72">
@@ -13713,43 +13713,43 @@
         <v>71.0</v>
       </c>
       <c r="B72" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="D72" s="2" t="n">
+        <v>776.0</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="F72" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G72" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H72" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="I72" s="2" t="n">
+        <v>1412.0</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="K72" s="2" t="n">
+        <v>918.0</v>
+      </c>
+      <c r="L72" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="D72" s="2" t="n">
-        <v>588.0</v>
-      </c>
-      <c r="E72" s="2" t="s">
+      <c r="M72" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N72" s="2" t="s">
         <v>359</v>
-      </c>
-      <c r="F72" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G72" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H72" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="I72" s="2" t="n">
-        <v>1320.0</v>
-      </c>
-      <c r="J72" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="K72" s="2" t="n">
-        <v>1065.0</v>
-      </c>
-      <c r="L72" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="M72" s="2" t="n">
-        <v>89.0</v>
-      </c>
-      <c r="N72" s="2" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="73">
@@ -13757,28 +13757,28 @@
         <v>72.0</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D73" s="2" t="n">
-        <v>349.0</v>
+        <v>588.0</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>362</v>
       </c>
       <c r="F73" s="2" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="G73" s="2" t="n">
-        <v>24.0</v>
+        <v>0.0</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I73" s="2" t="n">
-        <v>1326.0</v>
+        <v>1320.0</v>
       </c>
       <c r="J73" s="2" t="s">
         <v>363</v>
@@ -13787,13 +13787,13 @@
         <v>1065.0</v>
       </c>
       <c r="L73" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="M73" s="2" t="n">
+        <v>89.0</v>
+      </c>
+      <c r="N73" s="2" t="s">
         <v>364</v>
-      </c>
-      <c r="M73" s="2" t="n">
-        <v>95.0</v>
-      </c>
-      <c r="N73" s="2" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="74">
@@ -13801,43 +13801,43 @@
         <v>73.0</v>
       </c>
       <c r="B74" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="D74" s="2" t="n">
+        <v>349.0</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="F74" s="2" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="G74" s="2" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="I74" s="2" t="n">
+        <v>1326.0</v>
+      </c>
+      <c r="J74" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="K74" s="2" t="n">
+        <v>1065.0</v>
+      </c>
+      <c r="L74" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="D74" s="2" t="n">
-        <v>743.0</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="F74" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G74" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H74" s="2" t="s">
+      <c r="M74" s="2" t="n">
+        <v>95.0</v>
+      </c>
+      <c r="N74" s="2" t="s">
         <v>368</v>
-      </c>
-      <c r="I74" s="2" t="n">
-        <v>1418.0</v>
-      </c>
-      <c r="J74" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="K74" s="2" t="n">
-        <v>986.0</v>
-      </c>
-      <c r="L74" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="M74" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N74" s="2" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="75">
@@ -13845,43 +13845,43 @@
         <v>74.0</v>
       </c>
       <c r="B75" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="C75" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="D75" s="2" t="n">
+        <v>743.0</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F75" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G75" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H75" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="D75" s="2" t="n">
-        <v>660.0</v>
-      </c>
-      <c r="E75" s="2" t="s">
+      <c r="I75" s="2" t="n">
+        <v>1418.0</v>
+      </c>
+      <c r="J75" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="K75" s="2" t="n">
+        <v>986.0</v>
+      </c>
+      <c r="L75" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="M75" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N75" s="2" t="s">
         <v>372</v>
-      </c>
-      <c r="F75" s="2" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="G75" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H75" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="I75" s="2" t="n">
-        <v>1353.0</v>
-      </c>
-      <c r="J75" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="K75" s="2" t="n">
-        <v>1202.0</v>
-      </c>
-      <c r="L75" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="M75" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N75" s="2" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="76">
@@ -13889,16 +13889,16 @@
         <v>75.0</v>
       </c>
       <c r="B76" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="C76" s="2" t="s">
         <v>374</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>375</v>
       </c>
       <c r="D76" s="2" t="n">
         <v>772.0</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F76" s="2" t="n">
         <v>0.0</v>
@@ -13907,25 +13907,25 @@
         <v>0.0</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I76" s="2" t="n">
         <v>1353.0</v>
       </c>
       <c r="J76" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="K76" s="2" t="n">
         <v>836.0</v>
       </c>
       <c r="L76" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="M76" s="2" t="n">
         <v>14.0</v>
       </c>
       <c r="N76" s="2" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
     </row>
     <row r="77">
@@ -17166,7 +17166,7 @@
         <v>735</v>
       </c>
       <c r="I150" s="2" t="n">
-        <v>1562.0</v>
+        <v>1555.0</v>
       </c>
       <c r="J150" s="2" t="s">
         <v>736</v>
@@ -21287,10 +21287,10 @@
         <v>1194</v>
       </c>
       <c r="D244" s="2" t="n">
-        <v>0.0</v>
+        <v>343.0</v>
       </c>
       <c r="E244" s="2" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="F244" s="2" t="n">
         <v>0.0</v>
@@ -21299,25 +21299,25 @@
         <v>0.0</v>
       </c>
       <c r="H244" s="2" t="s">
-        <v>1194</v>
+        <v>194</v>
       </c>
       <c r="I244" s="2" t="n">
-        <v>1347.0</v>
+        <v>0.0</v>
       </c>
       <c r="J244" s="2" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="K244" s="2" t="n">
-        <v>1053.0</v>
+        <v>887.0</v>
       </c>
       <c r="L244" s="2" t="s">
-        <v>1194</v>
+        <v>1197</v>
       </c>
       <c r="M244" s="2" t="n">
-        <v>24.0</v>
+        <v>40.0</v>
       </c>
       <c r="N244" s="2" t="s">
-        <v>1196</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="245">
@@ -21325,16 +21325,16 @@
         <v>244.0</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>1197</v>
+        <v>1199</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>1198</v>
+        <v>194</v>
       </c>
       <c r="D245" s="2" t="n">
-        <v>343.0</v>
+        <v>0.0</v>
       </c>
       <c r="E245" s="2" t="s">
-        <v>1199</v>
+        <v>194</v>
       </c>
       <c r="F245" s="2" t="n">
         <v>0.0</v>
@@ -21343,25 +21343,25 @@
         <v>0.0</v>
       </c>
       <c r="H245" s="2" t="s">
-        <v>194</v>
+        <v>1200</v>
       </c>
       <c r="I245" s="2" t="n">
-        <v>0.0</v>
+        <v>1586.0</v>
       </c>
       <c r="J245" s="2" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="K245" s="2" t="n">
-        <v>887.0</v>
+        <v>984.0</v>
       </c>
       <c r="L245" s="2" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="M245" s="2" t="n">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
       <c r="N245" s="2" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="246">
@@ -21369,16 +21369,16 @@
         <v>245.0</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="C246" s="2" t="s">
-        <v>194</v>
+        <v>1205</v>
       </c>
       <c r="D246" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E246" s="2" t="s">
-        <v>194</v>
+        <v>1205</v>
       </c>
       <c r="F246" s="2" t="n">
         <v>0.0</v>
@@ -21387,25 +21387,25 @@
         <v>0.0</v>
       </c>
       <c r="H246" s="2" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="I246" s="2" t="n">
-        <v>1586.0</v>
+        <v>1452.0</v>
       </c>
       <c r="J246" s="2" t="s">
         <v>1205</v>
       </c>
       <c r="K246" s="2" t="n">
-        <v>984.0</v>
+        <v>1107.0</v>
       </c>
       <c r="L246" s="2" t="s">
+        <v>1205</v>
+      </c>
+      <c r="M246" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N246" s="2" t="s">
         <v>1206</v>
-      </c>
-      <c r="M246" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N246" s="2" t="s">
-        <v>1207</v>
       </c>
     </row>
     <row r="247">
@@ -21413,16 +21413,16 @@
         <v>246.0</v>
       </c>
       <c r="B247" s="2" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C247" s="2" t="s">
         <v>1208</v>
       </c>
-      <c r="C247" s="2" t="s">
-        <v>1209</v>
-      </c>
       <c r="D247" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E247" s="2" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="F247" s="2" t="n">
         <v>0.0</v>
@@ -21431,22 +21431,22 @@
         <v>0.0</v>
       </c>
       <c r="H247" s="2" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="I247" s="2" t="n">
-        <v>1452.0</v>
+        <v>1401.0</v>
       </c>
       <c r="J247" s="2" t="s">
         <v>1209</v>
       </c>
       <c r="K247" s="2" t="n">
-        <v>1107.0</v>
+        <v>1131.0</v>
       </c>
       <c r="L247" s="2" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="M247" s="2" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="N247" s="2" t="s">
         <v>1210</v>
@@ -21466,7 +21466,7 @@
         <v>0.0</v>
       </c>
       <c r="E248" s="2" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="F248" s="2" t="n">
         <v>0.0</v>
@@ -21475,25 +21475,25 @@
         <v>0.0</v>
       </c>
       <c r="H248" s="2" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="I248" s="2" t="n">
-        <v>1401.0</v>
+        <v>1487.0</v>
       </c>
       <c r="J248" s="2" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="K248" s="2" t="n">
-        <v>1131.0</v>
+        <v>1048.0</v>
       </c>
       <c r="L248" s="2" t="s">
         <v>1212</v>
       </c>
       <c r="M248" s="2" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="N248" s="2" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="249">
@@ -21501,16 +21501,16 @@
         <v>248.0</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="C249" s="2" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="D249" s="2" t="n">
         <v>0.0</v>
       </c>
       <c r="E249" s="2" t="s">
-        <v>1215</v>
+        <v>1217</v>
       </c>
       <c r="F249" s="2" t="n">
         <v>0.0</v>
@@ -21522,19 +21522,19 @@
         <v>1217</v>
       </c>
       <c r="I249" s="2" t="n">
-        <v>1487.0</v>
+        <v>1304.0</v>
       </c>
       <c r="J249" s="2" t="s">
         <v>1218</v>
       </c>
       <c r="K249" s="2" t="n">
-        <v>1048.0</v>
+        <v>1053.0</v>
       </c>
       <c r="L249" s="2" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="M249" s="2" t="n">
-        <v>2.0</v>
+        <v>24.0</v>
       </c>
       <c r="N249" s="2" t="s">
         <v>1219</v>
@@ -25024,13 +25024,13 @@
         <v>1596</v>
       </c>
       <c r="C329" s="2" t="s">
-        <v>194</v>
+        <v>1597</v>
       </c>
       <c r="D329" s="2" t="n">
-        <v>0.0</v>
+        <v>350.0</v>
       </c>
       <c r="E329" s="2" t="s">
-        <v>194</v>
+        <v>1597</v>
       </c>
       <c r="F329" s="2" t="n">
         <v>0.0</v>
@@ -25042,10 +25042,10 @@
         <v>1597</v>
       </c>
       <c r="I329" s="2" t="n">
-        <v>1423.0</v>
+        <v>0.0</v>
       </c>
       <c r="J329" s="2" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="K329" s="2" t="n">
         <v>0.0</v>
@@ -25057,7 +25057,7 @@
         <v>0.0</v>
       </c>
       <c r="N329" s="2" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="330">
@@ -25065,28 +25065,28 @@
         <v>329.0</v>
       </c>
       <c r="B330" s="2" t="s">
+        <v>1599</v>
+      </c>
+      <c r="C330" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D330" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E330" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F330" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G330" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H330" s="2" t="s">
         <v>1600</v>
       </c>
-      <c r="C330" s="2" t="s">
-        <v>1601</v>
-      </c>
-      <c r="D330" s="2" t="n">
-        <v>350.0</v>
-      </c>
-      <c r="E330" s="2" t="s">
-        <v>1601</v>
-      </c>
-      <c r="F330" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G330" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H330" s="2" t="s">
-        <v>1601</v>
-      </c>
       <c r="I330" s="2" t="n">
-        <v>0.0</v>
+        <v>1387.0</v>
       </c>
       <c r="J330" s="2" t="s">
         <v>1601</v>
@@ -25095,7 +25095,7 @@
         <v>0.0</v>
       </c>
       <c r="L330" s="2" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="M330" s="2" t="n">
         <v>0.0</v>

</xml_diff>

<commit_message>
Add generated leaderboard data - 2024-07-12T19:22:25
</commit_message>
<xml_diff>
--- a/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
+++ b/Leaderboards/CurrentCMRITLeaderboard2026.xlsx
@@ -170,7 +170,7 @@
     <t>cmr_22r01a05c9</t>
   </si>
   <si>
-    <t>53.32</t>
+    <t>54.21</t>
   </si>
   <si>
     <t>22R01A05E2</t>
@@ -479,6 +479,21 @@
     <t>40.95</t>
   </si>
   <si>
+    <t>22R01A05N4</t>
+  </si>
+  <si>
+    <t>mkeerthi63027</t>
+  </si>
+  <si>
+    <t>mkeerthify</t>
+  </si>
+  <si>
+    <t>keerthi_mangali</t>
+  </si>
+  <si>
+    <t>40.88</t>
+  </si>
+  <si>
     <t>22R01A66E8</t>
   </si>
   <si>
@@ -527,21 +542,6 @@
     <t>40.26</t>
   </si>
   <si>
-    <t>22R01A05N4</t>
-  </si>
-  <si>
-    <t>mkeerthi63027</t>
-  </si>
-  <si>
-    <t>mkeerthify</t>
-  </si>
-  <si>
-    <t>keerthi_mangali</t>
-  </si>
-  <si>
-    <t>40.13</t>
-  </si>
-  <si>
     <t>22R01A0474</t>
   </si>
   <si>
@@ -1526,7 +1526,7 @@
     <t>chef22r01a67a8</t>
   </si>
   <si>
-    <t>31.6</t>
+    <t>31.5</t>
   </si>
   <si>
     <t>22R01A0549</t>
@@ -4811,7 +4811,7 @@
     <t>Varsha_29</t>
   </si>
   <si>
-    <t>8.54</t>
+    <t>8.68</t>
   </si>
   <si>
     <t>23R05A0505</t>
@@ -10929,7 +10929,7 @@
         <v>50</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>932.0</v>
+        <v>968.0</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>50</v>
@@ -11897,7 +11897,7 @@
         <v>156</v>
       </c>
       <c r="D31" s="2" t="n">
-        <v>887.0</v>
+        <v>628.0</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>157</v>
@@ -11912,22 +11912,22 @@
         <v>158</v>
       </c>
       <c r="I31" s="2" t="n">
-        <v>1415.0</v>
+        <v>1487.0</v>
       </c>
       <c r="J31" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="K31" s="2" t="n">
+        <v>1082.0</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="M31" s="2" t="n">
+        <v>193.0</v>
+      </c>
+      <c r="N31" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="K31" s="2" t="n">
-        <v>1484.0</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="M31" s="2" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="N31" s="2" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="32">
@@ -11935,16 +11935,16 @@
         <v>31.0</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>887.0</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D32" s="2" t="n">
-        <v>891.0</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="F32" s="2" t="n">
         <v>0.0</v>
@@ -11956,19 +11956,19 @@
         <v>163</v>
       </c>
       <c r="I32" s="2" t="n">
-        <v>1369.0</v>
+        <v>1415.0</v>
       </c>
       <c r="J32" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K32" s="2" t="n">
+        <v>1484.0</v>
+      </c>
+      <c r="L32" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="K32" s="2" t="n">
-        <v>921.0</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>163</v>
-      </c>
       <c r="M32" s="2" t="n">
-        <v>83.0</v>
+        <v>5.0</v>
       </c>
       <c r="N32" s="2" t="s">
         <v>166</v>
@@ -11985,37 +11985,37 @@
         <v>168</v>
       </c>
       <c r="D33" s="2" t="n">
-        <v>850.0</v>
+        <v>891.0</v>
       </c>
       <c r="E33" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F33" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G33" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H33" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="F33" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G33" s="2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="I33" s="2" t="n">
-        <v>1412.0</v>
+        <v>1369.0</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K33" s="2" t="n">
-        <v>912.0</v>
+        <v>921.0</v>
       </c>
       <c r="L33" s="2" t="s">
         <v>168</v>
       </c>
       <c r="M33" s="2" t="n">
-        <v>95.0</v>
+        <v>83.0</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="34">
@@ -12023,13 +12023,13 @@
         <v>33.0</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D34" s="2" t="n">
-        <v>598.0</v>
+        <v>850.0</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>173</v>
@@ -12044,19 +12044,19 @@
         <v>174</v>
       </c>
       <c r="I34" s="2" t="n">
-        <v>1487.0</v>
+        <v>1412.0</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="K34" s="2" t="n">
-        <v>1082.0</v>
+        <v>912.0</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="M34" s="2" t="n">
-        <v>193.0</v>
+        <v>95.0</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>175</v>
@@ -15080,7 +15080,7 @@
         <v>502</v>
       </c>
       <c r="I103" s="2" t="n">
-        <v>1339.0</v>
+        <v>1323.0</v>
       </c>
       <c r="J103" s="2" t="s">
         <v>503</v>
@@ -25068,7 +25068,7 @@
         <v>1597</v>
       </c>
       <c r="I330" s="2" t="n">
-        <v>1387.0</v>
+        <v>1410.0</v>
       </c>
       <c r="J330" s="2" t="s">
         <v>1598</v>

</xml_diff>